<commit_message>
Update lab list for spring 2021
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2021spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2021spring.xlsx
@@ -1,27 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\131\StudentGuideModule1\what_labs_to_include\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9324" yWindow="456" windowWidth="49104" windowHeight="26724" tabRatio="539"/>
+    <workbookView xWindow="-4920" yWindow="0" windowWidth="30160" windowHeight="16120" tabRatio="539"/>
   </bookViews>
   <sheets>
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -33,7 +25,7 @@
     <author>Matt Trawick</author>
   </authors>
   <commentList>
-    <comment ref="W1" authorId="0" shapeId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X11" authorId="0" shapeId="0">
+    <comment ref="Z11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y19" authorId="0" shapeId="0">
+    <comment ref="AA19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -204,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W22" authorId="0" shapeId="0">
+    <comment ref="Y22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -237,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X22" authorId="0" shapeId="0">
+    <comment ref="Z22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -261,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z22" authorId="0" shapeId="0">
+    <comment ref="AB22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -286,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N61" authorId="0" shapeId="0">
+    <comment ref="N61" authorId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="212">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -947,16 +939,22 @@
   </si>
   <si>
     <t>Separated from Instrumentation 2020</t>
+  </si>
+  <si>
+    <t>2021 spr Mariama</t>
+  </si>
+  <si>
+    <t>2021 spr Haw</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1117,6 +1115,22 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1417,11 +1431,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1430,7 +1444,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1438,17 +1452,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1458,7 +1472,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1466,23 +1480,23 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1490,7 +1504,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1500,14 +1514,14 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1516,10 +1530,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1527,11 +1541,11 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1540,12 +1554,12 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1588,10 +1602,12 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1603,11 +1619,11 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1621,7 +1637,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1759,10 +1775,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1785,9 +1797,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1817,11 +1828,13 @@
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Currency" xfId="42" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1920,7 +1933,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1953,9 +1966,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1988,6 +2018,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2164,30 +2211,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD123"/>
+  <dimension ref="A1:AF123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="W50" sqref="W50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="13" customWidth="1"/>
-    <col min="4" max="8" width="5.77734375" style="13" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" style="19" customWidth="1"/>
-    <col min="10" max="11" width="10.109375" style="34" customWidth="1"/>
-    <col min="12" max="19" width="8.77734375" style="34" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="11" style="3" customWidth="1"/>
-    <col min="22" max="22" width="2.44140625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" style="3" customWidth="1"/>
-    <col min="25" max="25" width="9.44140625" customWidth="1"/>
-    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="13" customWidth="1"/>
+    <col min="4" max="8" width="5.83203125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="19" customWidth="1"/>
+    <col min="10" max="11" width="10.1640625" style="34" customWidth="1"/>
+    <col min="12" max="14" width="8.83203125" style="34" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="34" customWidth="1"/>
+    <col min="16" max="21" width="8.83203125" style="34" customWidth="1"/>
+    <col min="22" max="22" width="8.83203125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="11" style="3" customWidth="1"/>
+    <col min="24" max="24" width="2.5" style="3" customWidth="1"/>
+    <col min="25" max="25" width="10.33203125" style="3" customWidth="1"/>
+    <col min="27" max="27" width="9.5" customWidth="1"/>
+    <col min="28" max="28" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" s="1" customFormat="1" ht="28">
       <c r="A1" s="46" t="s">
         <v>73</v>
       </c>
@@ -2246,22 +2295,28 @@
         <v>205</v>
       </c>
       <c r="T1" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="U1" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="W1" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="V1" s="30"/>
-      <c r="W1" s="31"/>
       <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
+      <c r="Y1" s="31"/>
       <c r="Z1" s="30"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
       <c r="AC1" s="31"/>
       <c r="AD1" s="31"/>
-    </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+    </row>
+    <row r="2" spans="1:32" s="1" customFormat="1">
       <c r="A2" s="10" t="s">
         <v>86</v>
       </c>
@@ -2289,24 +2344,26 @@
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
       <c r="S2" s="56"/>
-      <c r="T2" s="53">
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="53">
         <v>3</v>
       </c>
-      <c r="U2" s="72">
-        <f>SUM(Q2:T2)</f>
+      <c r="W2" s="72">
+        <f>SUM(T2:V2)</f>
         <v>3</v>
       </c>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="73"/>
+      <c r="Z2" s="73"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="30"/>
       <c r="AC2" s="31"/>
       <c r="AD2" s="31"/>
-    </row>
-    <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="31"/>
+    </row>
+    <row r="3" spans="1:32" s="1" customFormat="1">
       <c r="A3" s="46"/>
       <c r="B3" s="52" t="s">
         <v>88</v>
@@ -2332,24 +2389,26 @@
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
       <c r="S3" s="57"/>
-      <c r="T3" s="57">
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57">
         <v>3</v>
       </c>
-      <c r="U3" s="73">
-        <f t="shared" ref="U3:U67" si="0">SUM(Q3:T3)</f>
+      <c r="W3" s="72">
+        <f t="shared" ref="W3:W66" si="0">SUM(T3:V3)</f>
         <v>3</v>
       </c>
-      <c r="V3" s="75"/>
-      <c r="W3" s="75"/>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="75"/>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="31"/>
-      <c r="AB3" s="31"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="73"/>
+      <c r="Z3" s="73"/>
+      <c r="AA3" s="73"/>
+      <c r="AB3" s="30"/>
       <c r="AC3" s="31"/>
       <c r="AD3" s="31"/>
-    </row>
-    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="31"/>
+    </row>
+    <row r="4" spans="1:32" s="1" customFormat="1">
       <c r="A4" s="28" t="s">
         <v>110</v>
       </c>
@@ -2391,22 +2450,26 @@
       <c r="Q4" s="34"/>
       <c r="R4" s="34"/>
       <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="74">
+      <c r="T4" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="72">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
+        <v>0.5</v>
+      </c>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="31"/>
-      <c r="AB4" s="31"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="14"/>
       <c r="AC4" s="31"/>
       <c r="AD4" s="31"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="31"/>
+    </row>
+    <row r="5" spans="1:32">
       <c r="B5" s="22" t="s">
         <v>120</v>
       </c>
@@ -2420,22 +2483,22 @@
       <c r="N5" s="34">
         <v>0</v>
       </c>
-      <c r="T5" s="32"/>
-      <c r="U5" s="74">
+      <c r="V5" s="32"/>
+      <c r="W5" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="31"/>
-      <c r="AB5" s="31"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="14"/>
       <c r="AC5" s="31"/>
       <c r="AD5" s="31"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE5" s="31"/>
+      <c r="AF5" s="31"/>
+    </row>
+    <row r="6" spans="1:32">
       <c r="A6" s="28"/>
       <c r="B6" s="29" t="s">
         <v>121</v>
@@ -2447,22 +2510,22 @@
       <c r="N6" s="34">
         <v>0</v>
       </c>
-      <c r="T6" s="34"/>
-      <c r="U6" s="74">
+      <c r="V6" s="34"/>
+      <c r="W6" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="31"/>
-      <c r="AB6" s="31"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="14"/>
       <c r="AC6" s="31"/>
       <c r="AD6" s="31"/>
-    </row>
-    <row r="7" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE6" s="31"/>
+      <c r="AF6" s="31"/>
+    </row>
+    <row r="7" spans="1:32" s="31" customFormat="1">
       <c r="A7" s="10"/>
       <c r="B7" s="22" t="s">
         <v>122</v>
@@ -2488,18 +2551,20 @@
       <c r="Q7" s="34"/>
       <c r="R7" s="34"/>
       <c r="S7" s="34"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="74">
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
-      <c r="Z7" s="14"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="14"/>
+    </row>
+    <row r="8" spans="1:32">
       <c r="B8" s="22" t="s">
         <v>123</v>
       </c>
@@ -2510,22 +2575,22 @@
       <c r="N8" s="34">
         <v>0</v>
       </c>
-      <c r="T8" s="32"/>
-      <c r="U8" s="74">
+      <c r="V8" s="32"/>
+      <c r="W8" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="31"/>
-      <c r="AB8" s="31"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="14"/>
       <c r="AC8" s="31"/>
       <c r="AD8" s="31"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE8" s="31"/>
+      <c r="AF8" s="31"/>
+    </row>
+    <row r="9" spans="1:32">
       <c r="B9" s="22" t="s">
         <v>124</v>
       </c>
@@ -2569,22 +2634,31 @@
       <c r="R9" s="34">
         <v>1</v>
       </c>
-      <c r="T9" s="32"/>
-      <c r="U9" s="74">
+      <c r="S9" s="34">
+        <v>1</v>
+      </c>
+      <c r="T9" s="34">
+        <v>1</v>
+      </c>
+      <c r="U9" s="34">
+        <v>1</v>
+      </c>
+      <c r="V9" s="32"/>
+      <c r="W9" s="72">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="31"/>
-      <c r="AB9" s="31"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="14"/>
       <c r="AC9" s="31"/>
       <c r="AD9" s="31"/>
-    </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE9" s="31"/>
+      <c r="AF9" s="31"/>
+    </row>
+    <row r="10" spans="1:32" ht="15" thickBot="1">
       <c r="B10" s="22" t="s">
         <v>125</v>
       </c>
@@ -2628,22 +2702,31 @@
       <c r="R10" s="34">
         <v>1</v>
       </c>
-      <c r="T10" s="32"/>
-      <c r="U10" s="74">
+      <c r="S10" s="34">
+        <v>1</v>
+      </c>
+      <c r="T10" s="34">
+        <v>1</v>
+      </c>
+      <c r="U10" s="34">
+        <v>1</v>
+      </c>
+      <c r="V10" s="32"/>
+      <c r="W10" s="72">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="31"/>
-      <c r="AB10" s="31"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="14"/>
       <c r="AC10" s="31"/>
       <c r="AD10" s="31"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="31"/>
+    </row>
+    <row r="11" spans="1:32">
       <c r="B11" s="22" t="s">
         <v>126</v>
       </c>
@@ -2684,24 +2767,33 @@
       <c r="R11" s="34">
         <v>1</v>
       </c>
-      <c r="T11" s="32"/>
-      <c r="U11" s="74">
+      <c r="S11" s="34">
+        <v>1</v>
+      </c>
+      <c r="T11" s="34">
+        <v>1</v>
+      </c>
+      <c r="U11" s="34">
+        <v>1</v>
+      </c>
+      <c r="V11" s="32"/>
+      <c r="W11" s="72">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="V11" s="5"/>
-      <c r="W11" s="40" t="s">
+      <c r="X11" s="5"/>
+      <c r="Y11" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="31"/>
-      <c r="AB11" s="31"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="14"/>
       <c r="AC11" s="31"/>
       <c r="AD11" s="31"/>
-    </row>
-    <row r="12" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE11" s="31"/>
+      <c r="AF11" s="31"/>
+    </row>
+    <row r="12" spans="1:32" ht="15" thickBot="1">
       <c r="B12" s="22" t="s">
         <v>127</v>
       </c>
@@ -2712,24 +2804,24 @@
       <c r="N12" s="34">
         <v>0</v>
       </c>
-      <c r="T12" s="32"/>
-      <c r="U12" s="74">
+      <c r="V12" s="32"/>
+      <c r="W12" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V12" s="14"/>
-      <c r="W12" s="42">
-        <v>1</v>
-      </c>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="31"/>
-      <c r="AB12" s="31"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="14"/>
       <c r="AC12" s="31"/>
       <c r="AD12" s="31"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="31"/>
+    </row>
+    <row r="13" spans="1:32">
       <c r="B13" s="22" t="s">
         <v>175</v>
       </c>
@@ -2770,22 +2862,25 @@
       <c r="R13" s="34">
         <v>1</v>
       </c>
-      <c r="T13" s="32"/>
-      <c r="U13" s="74">
+      <c r="T13" s="34">
+        <v>1</v>
+      </c>
+      <c r="V13" s="32"/>
+      <c r="W13" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V13" s="5"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="31"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="31"/>
-      <c r="AB13" s="31"/>
+        <v>1</v>
+      </c>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="31"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="14"/>
       <c r="AC13" s="31"/>
       <c r="AD13" s="31"/>
-    </row>
-    <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE13" s="31"/>
+      <c r="AF13" s="31"/>
+    </row>
+    <row r="14" spans="1:32" ht="15" thickBot="1">
       <c r="B14" s="22" t="s">
         <v>128</v>
       </c>
@@ -2826,23 +2921,26 @@
       <c r="R14" s="34">
         <v>1</v>
       </c>
-      <c r="T14" s="32"/>
-      <c r="U14" s="74">
+      <c r="T14" s="34">
+        <v>1</v>
+      </c>
+      <c r="V14" s="32"/>
+      <c r="W14" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V14" s="5"/>
-      <c r="W14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Y14" s="31"/>
-      <c r="Z14" s="14"/>
       <c r="AA14" s="31"/>
-      <c r="AB14" s="31"/>
+      <c r="AB14" s="14"/>
       <c r="AC14" s="31"/>
       <c r="AD14" s="31"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="31"/>
+    </row>
+    <row r="15" spans="1:32">
       <c r="B15" s="22" t="s">
         <v>174</v>
       </c>
@@ -2859,26 +2957,26 @@
       <c r="O15" s="34">
         <v>0.5</v>
       </c>
-      <c r="T15" s="32"/>
-      <c r="U15" s="74">
+      <c r="V15" s="32"/>
+      <c r="W15" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V15" s="5"/>
-      <c r="W15" s="16" t="s">
+      <c r="X15" s="5"/>
+      <c r="Y15" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="X15" s="36"/>
-      <c r="Y15" s="15">
+      <c r="Z15" s="36"/>
+      <c r="AA15" s="15">
         <v>0.05</v>
       </c>
-      <c r="Z15" s="31"/>
-      <c r="AA15" s="31"/>
       <c r="AB15" s="31"/>
       <c r="AC15" s="31"/>
       <c r="AD15" s="31"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE15" s="31"/>
+      <c r="AF15" s="31"/>
+    </row>
+    <row r="16" spans="1:32">
       <c r="B16" s="22" t="s">
         <v>129</v>
       </c>
@@ -2895,26 +2993,26 @@
       <c r="O16" s="34">
         <v>0.5</v>
       </c>
-      <c r="T16" s="32"/>
-      <c r="U16" s="74">
+      <c r="V16" s="32"/>
+      <c r="W16" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V16" s="5"/>
-      <c r="W16" s="17" t="s">
+      <c r="X16" s="5"/>
+      <c r="Y16" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="8">
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="8">
         <v>0.3</v>
       </c>
-      <c r="Z16" s="31"/>
-      <c r="AA16" s="31"/>
       <c r="AB16" s="31"/>
       <c r="AC16" s="31"/>
       <c r="AD16" s="31"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE16" s="31"/>
+      <c r="AF16" s="31"/>
+    </row>
+    <row r="17" spans="1:32">
       <c r="B17" s="22" t="s">
         <v>130</v>
       </c>
@@ -2946,26 +3044,29 @@
       <c r="Q17" s="34">
         <v>1</v>
       </c>
-      <c r="T17" s="32"/>
-      <c r="U17" s="74">
+      <c r="T17" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="V17" s="32"/>
+      <c r="W17" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V17" s="5"/>
-      <c r="W17" s="17" t="s">
+        <v>0.75</v>
+      </c>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="8">
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="8">
         <v>3</v>
       </c>
-      <c r="Z17" s="31"/>
-      <c r="AA17" s="31"/>
       <c r="AB17" s="31"/>
       <c r="AC17" s="31"/>
       <c r="AD17" s="31"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE17" s="31"/>
+      <c r="AF17" s="31"/>
+    </row>
+    <row r="18" spans="1:32">
       <c r="B18" s="22" t="s">
         <v>131</v>
       </c>
@@ -3006,26 +3107,29 @@
       <c r="Q18" s="34">
         <v>1</v>
       </c>
-      <c r="T18" s="32"/>
-      <c r="U18" s="74">
+      <c r="T18" s="34">
+        <v>1</v>
+      </c>
+      <c r="V18" s="32"/>
+      <c r="W18" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V18" s="5"/>
-      <c r="W18" s="17" t="s">
+      <c r="X18" s="5"/>
+      <c r="Y18" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="37">
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="37">
         <v>0.25</v>
       </c>
-      <c r="Z18" s="31"/>
-      <c r="AA18" s="31"/>
       <c r="AB18" s="31"/>
       <c r="AC18" s="31"/>
       <c r="AD18" s="31"/>
-    </row>
-    <row r="19" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="31"/>
+    </row>
+    <row r="19" spans="1:32" ht="15" thickBot="1">
       <c r="B19" s="22" t="s">
         <v>132</v>
       </c>
@@ -3039,26 +3143,26 @@
       <c r="R19" s="34">
         <v>1</v>
       </c>
-      <c r="T19" s="32"/>
-      <c r="U19" s="74">
+      <c r="V19" s="32"/>
+      <c r="W19" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V19" s="14"/>
-      <c r="W19" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="39">
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="39">
         <v>0.05</v>
       </c>
-      <c r="Z19" s="31"/>
-      <c r="AA19" s="31"/>
       <c r="AB19" s="31"/>
       <c r="AC19" s="31"/>
       <c r="AD19" s="31"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE19" s="31"/>
+      <c r="AF19" s="31"/>
+    </row>
+    <row r="20" spans="1:32">
       <c r="B20" s="22" t="s">
         <v>133</v>
       </c>
@@ -3069,19 +3173,19 @@
       <c r="N20" s="34">
         <v>0.5</v>
       </c>
-      <c r="T20" s="32"/>
-      <c r="U20" s="74">
+      <c r="V20" s="32"/>
+      <c r="W20" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V20" s="14"/>
-      <c r="Z20" s="31"/>
-      <c r="AA20" s="31"/>
+      <c r="X20" s="14"/>
       <c r="AB20" s="31"/>
       <c r="AC20" s="31"/>
       <c r="AD20" s="31"/>
-    </row>
-    <row r="21" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE20" s="31"/>
+      <c r="AF20" s="31"/>
+    </row>
+    <row r="21" spans="1:32" ht="15" thickBot="1">
       <c r="B21" s="22" t="s">
         <v>134</v>
       </c>
@@ -3092,22 +3196,22 @@
       <c r="N21" s="34">
         <v>0</v>
       </c>
-      <c r="T21" s="32"/>
-      <c r="U21" s="74">
+      <c r="V21" s="32"/>
+      <c r="W21" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="31"/>
-      <c r="AA21" s="31"/>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="14"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
       <c r="AB21" s="31"/>
       <c r="AC21" s="31"/>
       <c r="AD21" s="31"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE21" s="31"/>
+      <c r="AF21" s="31"/>
+    </row>
+    <row r="22" spans="1:32">
       <c r="B22" s="22" t="s">
         <v>135</v>
       </c>
@@ -3118,30 +3222,30 @@
       <c r="N22" s="34">
         <v>0.1</v>
       </c>
-      <c r="T22" s="32"/>
-      <c r="U22" s="74">
+      <c r="V22" s="32"/>
+      <c r="W22" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V22" s="14"/>
-      <c r="W22" s="44" t="s">
+      <c r="X22" s="14"/>
+      <c r="Y22" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="X22" s="4" t="s">
+      <c r="Z22" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="Y22" s="4" t="s">
+      <c r="AA22" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="Z22" s="7" t="s">
+      <c r="AB22" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="31"/>
       <c r="AC22" s="31"/>
       <c r="AD22" s="31"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE22" s="31"/>
+      <c r="AF22" s="31"/>
+    </row>
+    <row r="23" spans="1:32">
       <c r="B23" s="22" t="s">
         <v>136</v>
       </c>
@@ -3152,33 +3256,33 @@
       <c r="N23" s="34">
         <v>0</v>
       </c>
-      <c r="T23" s="32"/>
-      <c r="U23" s="74">
+      <c r="V23" s="32"/>
+      <c r="W23" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V23" s="14"/>
-      <c r="W23" s="76">
+      <c r="X23" s="14"/>
+      <c r="Y23" s="74">
         <v>0</v>
       </c>
-      <c r="X23" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W23,C$2:C$82)</f>
+      <c r="Z23" s="6">
+        <f t="shared" ref="Z23:Z31" si="1">SUMIF(W$2:W$82,"&gt;=" &amp; Y23,C$2:C$82)</f>
         <v>330</v>
       </c>
-      <c r="Y23" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W23,D$2:D$82)</f>
+      <c r="AA23" s="6">
+        <f t="shared" ref="AA23:AA31" si="2">SUMIF(W$2:W$82,"&gt;=" &amp; Y23,D$2:D$82)</f>
         <v>11</v>
       </c>
-      <c r="Z23" s="8">
-        <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
+      <c r="AB23" s="8">
+        <f t="shared" ref="AB23:AB31" si="3">($AA$17 + $AA$15*Z23+$AA$16*AA23)*(1+AA$18+AA$19)</f>
         <v>29.64</v>
       </c>
-      <c r="AA23" s="31"/>
-      <c r="AB23" s="31"/>
       <c r="AC23" s="31"/>
       <c r="AD23" s="31"/>
-    </row>
-    <row r="24" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE23" s="31"/>
+      <c r="AF23" s="31"/>
+    </row>
+    <row r="24" spans="1:32" s="6" customFormat="1">
       <c r="A24" s="10"/>
       <c r="B24" s="22" t="s">
         <v>137</v>
@@ -3225,34 +3329,42 @@
       <c r="R24" s="34">
         <v>1</v>
       </c>
-      <c r="S24" s="34"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="74">
+      <c r="S24" s="34">
+        <v>1</v>
+      </c>
+      <c r="T24" s="34">
+        <v>1</v>
+      </c>
+      <c r="U24" s="34">
+        <v>1</v>
+      </c>
+      <c r="V24" s="32"/>
+      <c r="W24" s="72">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="V24" s="14"/>
-      <c r="W24" s="76">
+      <c r="X24" s="14"/>
+      <c r="Y24" s="74">
         <v>0.5</v>
       </c>
-      <c r="X24" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W24,C$2:C$82)</f>
-        <v>242</v>
-      </c>
-      <c r="Y24" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W24,D$2:D$82)</f>
-        <v>10</v>
-      </c>
-      <c r="Z24" s="8">
+      <c r="Z24" s="6">
         <f t="shared" si="1"/>
-        <v>23.53</v>
-      </c>
-      <c r="AA24" s="31"/>
-      <c r="AB24" s="31"/>
+        <v>234</v>
+      </c>
+      <c r="AA24" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="AB24" s="8">
+        <f t="shared" si="3"/>
+        <v>21.060000000000006</v>
+      </c>
       <c r="AC24" s="31"/>
       <c r="AD24" s="31"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE24" s="31"/>
+      <c r="AF24" s="31"/>
+    </row>
+    <row r="25" spans="1:32">
       <c r="B25" s="22" t="s">
         <v>138</v>
       </c>
@@ -3280,35 +3392,38 @@
       <c r="P25" s="34">
         <v>1</v>
       </c>
-      <c r="T25" s="32">
-        <v>1</v>
-      </c>
-      <c r="U25" s="74">
+      <c r="T25" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="V25" s="32">
+        <v>1</v>
+      </c>
+      <c r="W25" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V25" s="14"/>
-      <c r="W25" s="76">
-        <v>1</v>
-      </c>
-      <c r="X25" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W25,C$2:C$82)</f>
-        <v>236</v>
-      </c>
-      <c r="Y25" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W25,D$2:D$82)</f>
-        <v>10</v>
-      </c>
-      <c r="Z25" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="74">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="6">
         <f t="shared" si="1"/>
-        <v>23.14</v>
-      </c>
-      <c r="AA25" s="31"/>
-      <c r="AB25" s="31"/>
+        <v>180</v>
+      </c>
+      <c r="AA25" s="6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AB25" s="8">
+        <f t="shared" si="3"/>
+        <v>16.38</v>
+      </c>
       <c r="AC25" s="31"/>
       <c r="AD25" s="31"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE25" s="31"/>
+      <c r="AF25" s="31"/>
+    </row>
+    <row r="26" spans="1:32">
       <c r="B26" s="22" t="s">
         <v>139</v>
       </c>
@@ -3346,33 +3461,36 @@
       <c r="Q26" s="34">
         <v>1</v>
       </c>
-      <c r="T26" s="32"/>
-      <c r="U26" s="83">
+      <c r="T26" s="34">
+        <v>1</v>
+      </c>
+      <c r="V26" s="32"/>
+      <c r="W26" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V26" s="14"/>
-      <c r="W26" s="77">
+      <c r="X26" s="14"/>
+      <c r="Y26" s="75">
         <v>1.5</v>
       </c>
-      <c r="X26" s="29">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W26,C$2:C$82)</f>
-        <v>124</v>
-      </c>
-      <c r="Y26" s="29">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W26,D$2:D$82)</f>
-        <v>2</v>
-      </c>
-      <c r="Z26" s="8">
+      <c r="Z26" s="29">
         <f t="shared" si="1"/>
-        <v>12.739999999999998</v>
-      </c>
-      <c r="AA26" s="31"/>
-      <c r="AB26" s="31"/>
+        <v>41</v>
+      </c>
+      <c r="AA26" s="29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AB26" s="8">
+        <f t="shared" si="3"/>
+        <v>6.955000000000001</v>
+      </c>
       <c r="AC26" s="31"/>
       <c r="AD26" s="31"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE26" s="31"/>
+      <c r="AF26" s="31"/>
+    </row>
+    <row r="27" spans="1:32">
       <c r="A27" s="11" t="s">
         <v>117</v>
       </c>
@@ -3422,29 +3540,33 @@
         <v>1</v>
       </c>
       <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="74">
+      <c r="T27" s="33">
+        <v>1</v>
+      </c>
+      <c r="U27" s="33"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="72">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X27" s="14"/>
+      <c r="Y27" s="74">
         <v>2</v>
       </c>
-      <c r="V27" s="14"/>
-      <c r="W27" s="76">
-        <v>2</v>
-      </c>
-      <c r="X27" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W27,C$2:C$82)</f>
-        <v>113</v>
-      </c>
-      <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W27,D$2:D$82)</f>
-        <v>2</v>
-      </c>
-      <c r="Z27" s="8">
+      <c r="Z27" s="6">
         <f t="shared" si="1"/>
-        <v>12.025</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="AA27" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AB27" s="8">
+        <f t="shared" si="3"/>
+        <v>6.6949999999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32">
       <c r="B28" s="22" t="s">
         <v>141</v>
       </c>
@@ -3482,29 +3604,32 @@
       <c r="R28" s="34">
         <v>1</v>
       </c>
-      <c r="T28" s="32"/>
-      <c r="U28" s="74">
+      <c r="T28" s="34">
+        <v>1</v>
+      </c>
+      <c r="V28" s="32"/>
+      <c r="W28" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V28" s="14"/>
-      <c r="W28" s="76">
+        <v>1</v>
+      </c>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="74">
         <v>2.5</v>
       </c>
-      <c r="X28" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W28,C$2:C$82)</f>
-        <v>6</v>
-      </c>
-      <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W28,D$2:D$82)</f>
-        <v>1</v>
-      </c>
-      <c r="Z28" s="8">
+      <c r="Z28" s="6">
         <f t="shared" si="1"/>
-        <v>4.68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="AA28" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AB28" s="8">
+        <f t="shared" si="3"/>
+        <v>5.0049999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32">
       <c r="B29" s="22" t="s">
         <v>142</v>
       </c>
@@ -3524,29 +3649,32 @@
       <c r="P29" s="34">
         <v>0.75</v>
       </c>
-      <c r="T29" s="32"/>
-      <c r="U29" s="74">
+      <c r="T29" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="V29" s="32"/>
+      <c r="W29" s="72">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V29" s="14"/>
-      <c r="W29" s="76">
+        <v>0.5</v>
+      </c>
+      <c r="X29" s="14"/>
+      <c r="Y29" s="74">
         <v>3</v>
       </c>
-      <c r="X29" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W29,C$2:C$82)</f>
-        <v>6</v>
-      </c>
-      <c r="Y29" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W29,D$2:D$82)</f>
-        <v>1</v>
-      </c>
-      <c r="Z29" s="8">
+      <c r="Z29" s="6">
         <f t="shared" si="1"/>
-        <v>4.68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="AA29" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AB29" s="8">
+        <f t="shared" si="3"/>
+        <v>5.0049999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32">
       <c r="B30" s="22" t="s">
         <v>143</v>
       </c>
@@ -3584,29 +3712,32 @@
       <c r="R30" s="34">
         <v>1</v>
       </c>
-      <c r="T30" s="32"/>
-      <c r="U30" s="74">
+      <c r="T30" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="V30" s="32"/>
+      <c r="W30" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V30" s="14"/>
-      <c r="W30" s="76">
+        <v>0.75</v>
+      </c>
+      <c r="X30" s="14"/>
+      <c r="Y30" s="74">
         <v>3.5</v>
       </c>
-      <c r="X30" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W30,C$2:C$82)</f>
+      <c r="Z30" s="6">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W30,D$2:D$82)</f>
+      <c r="AA30" s="6">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z30" s="8">
-        <f t="shared" si="1"/>
+      <c r="AB30" s="8">
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:32" ht="15" thickBot="1">
       <c r="B31" s="22" t="s">
         <v>191</v>
       </c>
@@ -3625,29 +3756,32 @@
       <c r="P31" s="34">
         <v>1</v>
       </c>
-      <c r="T31" s="32"/>
-      <c r="U31" s="74">
+      <c r="T31" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="V31" s="32"/>
+      <c r="W31" s="72">
         <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="76">
+        <v>4</v>
+      </c>
+      <c r="Z31" s="45">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V31" s="14"/>
-      <c r="W31" s="78">
-        <v>4</v>
-      </c>
-      <c r="X31" s="45">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W31,C$2:C$82)</f>
+      <c r="AA31" s="45">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y31" s="45">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W31,D$2:D$82)</f>
-        <v>0</v>
-      </c>
-      <c r="Z31" s="9">
-        <f t="shared" si="1"/>
+      <c r="AB31" s="9">
+        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" s="6" customFormat="1">
       <c r="A32" s="10"/>
       <c r="B32" s="22" t="s">
         <v>144</v>
@@ -3693,17 +3827,21 @@
       </c>
       <c r="R32" s="34"/>
       <c r="S32" s="34"/>
-      <c r="T32" s="32"/>
-      <c r="U32" s="74">
+      <c r="T32" s="34">
+        <v>1</v>
+      </c>
+      <c r="U32" s="34"/>
+      <c r="V32" s="32"/>
+      <c r="W32" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V32" s="14"/>
-      <c r="W32" s="3"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X32" s="14"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32"/>
+      <c r="AA32"/>
+    </row>
+    <row r="33" spans="1:32">
       <c r="B33" s="22" t="s">
         <v>145</v>
       </c>
@@ -3726,14 +3864,17 @@
       <c r="R33" s="34">
         <v>1</v>
       </c>
-      <c r="T33" s="32"/>
-      <c r="U33" s="74">
+      <c r="T33" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="V33" s="32"/>
+      <c r="W33" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V33" s="14"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="X33" s="14"/>
+    </row>
+    <row r="34" spans="1:32">
       <c r="B34" s="22" t="s">
         <v>146</v>
       </c>
@@ -3774,14 +3915,17 @@
       <c r="Q34" s="34">
         <v>1</v>
       </c>
-      <c r="T34" s="32"/>
-      <c r="U34" s="74">
+      <c r="T34" s="34">
+        <v>1</v>
+      </c>
+      <c r="V34" s="32"/>
+      <c r="W34" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V34" s="14"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X34" s="14"/>
+    </row>
+    <row r="35" spans="1:32">
       <c r="B35" s="22" t="s">
         <v>147</v>
       </c>
@@ -3803,17 +3947,17 @@
       <c r="N35" s="34">
         <v>1</v>
       </c>
-      <c r="T35" s="32">
-        <v>1</v>
-      </c>
-      <c r="U35" s="74">
+      <c r="V35" s="32">
+        <v>1</v>
+      </c>
+      <c r="W35" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V35" s="14"/>
-      <c r="W35" s="79"/>
-    </row>
-    <row r="36" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X35" s="14"/>
+      <c r="Y35" s="77"/>
+    </row>
+    <row r="36" spans="1:32" s="31" customFormat="1">
       <c r="A36" s="10"/>
       <c r="B36" s="22" t="s">
         <v>194</v>
@@ -3843,15 +3987,17 @@
         <v>1</v>
       </c>
       <c r="S36" s="34"/>
-      <c r="T36" s="32"/>
-      <c r="U36" s="74">
+      <c r="T36" s="34"/>
+      <c r="U36" s="34"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V36" s="14"/>
-      <c r="W36" s="79"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="77"/>
+    </row>
+    <row r="37" spans="1:32">
       <c r="B37" s="22" t="s">
         <v>148</v>
       </c>
@@ -3889,15 +4035,18 @@
       <c r="Q37" s="34">
         <v>1</v>
       </c>
-      <c r="T37" s="32"/>
-      <c r="U37" s="74">
+      <c r="T37" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="V37" s="32"/>
+      <c r="W37" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V37" s="14"/>
-      <c r="W37" s="79"/>
-    </row>
-    <row r="38" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="77"/>
+    </row>
+    <row r="38" spans="1:32" s="31" customFormat="1">
       <c r="A38" s="10"/>
       <c r="B38" s="22" t="s">
         <v>149</v>
@@ -3941,15 +4090,19 @@
       </c>
       <c r="R38" s="34"/>
       <c r="S38" s="34"/>
-      <c r="T38" s="32"/>
-      <c r="U38" s="74">
+      <c r="T38" s="34">
+        <v>1</v>
+      </c>
+      <c r="U38" s="34"/>
+      <c r="V38" s="32"/>
+      <c r="W38" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V38" s="14"/>
-      <c r="W38" s="79"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X38" s="14"/>
+      <c r="Y38" s="77"/>
+    </row>
+    <row r="39" spans="1:32">
       <c r="B39" s="22" t="s">
         <v>150</v>
       </c>
@@ -3978,16 +4131,16 @@
       <c r="O39" s="34">
         <v>0.5</v>
       </c>
-      <c r="T39" s="32"/>
-      <c r="U39" s="74">
+      <c r="V39" s="32"/>
+      <c r="W39" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V39" s="14"/>
-      <c r="W39" s="79"/>
-      <c r="Z39" s="6"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X39" s="14"/>
+      <c r="Y39" s="77"/>
+      <c r="AB39" s="6"/>
+    </row>
+    <row r="40" spans="1:32">
       <c r="B40" s="22" t="s">
         <v>180</v>
       </c>
@@ -4003,14 +4156,14 @@
       <c r="N40" s="34">
         <v>0</v>
       </c>
-      <c r="T40" s="32"/>
-      <c r="U40" s="83">
+      <c r="V40" s="32"/>
+      <c r="W40" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V40" s="14"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X40" s="14"/>
+    </row>
+    <row r="41" spans="1:32">
       <c r="A41" s="11" t="s">
         <v>116</v>
       </c>
@@ -4060,16 +4213,20 @@
       </c>
       <c r="R41" s="33"/>
       <c r="S41" s="33"/>
-      <c r="T41" s="33"/>
-      <c r="U41" s="74">
+      <c r="T41" s="33">
+        <v>0.75</v>
+      </c>
+      <c r="U41" s="33"/>
+      <c r="V41" s="33"/>
+      <c r="W41" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V41" s="14"/>
-      <c r="W41" s="14"/>
-      <c r="X41" s="6"/>
-    </row>
-    <row r="42" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0.75</v>
+      </c>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="14"/>
+      <c r="Z41" s="6"/>
+    </row>
+    <row r="42" spans="1:32" s="6" customFormat="1">
       <c r="A42" s="28"/>
       <c r="B42" s="29" t="s">
         <v>152</v>
@@ -4119,21 +4276,25 @@
         <v>1</v>
       </c>
       <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
-      <c r="U42" s="74">
+      <c r="T42" s="34">
+        <v>1</v>
+      </c>
+      <c r="U42" s="34"/>
+      <c r="V42" s="34"/>
+      <c r="W42" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V42" s="14"/>
-      <c r="W42" s="3"/>
-      <c r="X42"/>
-      <c r="Y42"/>
+        <v>1</v>
+      </c>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42"/>
       <c r="AA42"/>
-      <c r="AB42"/>
       <c r="AC42"/>
       <c r="AD42"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE42"/>
+      <c r="AF42"/>
+    </row>
+    <row r="43" spans="1:32">
       <c r="A43" s="28"/>
       <c r="B43" s="29" t="s">
         <v>153</v>
@@ -4175,18 +4336,27 @@
       <c r="Q43" s="34">
         <v>1</v>
       </c>
-      <c r="T43" s="34"/>
-      <c r="U43" s="74">
+      <c r="S43" s="34">
+        <v>1</v>
+      </c>
+      <c r="T43" s="34">
+        <v>1</v>
+      </c>
+      <c r="U43" s="34">
+        <v>1</v>
+      </c>
+      <c r="V43" s="34"/>
+      <c r="W43" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V43" s="14"/>
-      <c r="AA43" s="6"/>
-      <c r="AB43" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="X43" s="14"/>
       <c r="AC43" s="6"/>
       <c r="AD43" s="6"/>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE43" s="6"/>
+      <c r="AF43" s="6"/>
+    </row>
+    <row r="44" spans="1:32">
       <c r="A44" s="28"/>
       <c r="B44" s="29" t="s">
         <v>154</v>
@@ -4207,15 +4377,15 @@
       <c r="Q44" s="34">
         <v>0.5</v>
       </c>
-      <c r="T44" s="34"/>
-      <c r="U44" s="74">
+      <c r="V44" s="34"/>
+      <c r="W44" s="72">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="V44" s="14"/>
-      <c r="Z44" s="6"/>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="X44" s="14"/>
+      <c r="AB44" s="6"/>
+    </row>
+    <row r="45" spans="1:32">
       <c r="A45" s="28"/>
       <c r="B45" s="29" t="s">
         <v>155</v>
@@ -4251,16 +4421,16 @@
       <c r="O45" s="34">
         <v>1</v>
       </c>
-      <c r="T45" s="34"/>
-      <c r="U45" s="74">
+      <c r="V45" s="34"/>
+      <c r="W45" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V45" s="14"/>
-      <c r="W45" s="14"/>
-      <c r="X45" s="6"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X45" s="14"/>
+      <c r="Y45" s="14"/>
+      <c r="Z45" s="6"/>
+    </row>
+    <row r="46" spans="1:32">
       <c r="A46" s="28"/>
       <c r="B46" s="29" t="s">
         <v>156</v>
@@ -4302,15 +4472,18 @@
       <c r="R46" s="34">
         <v>1</v>
       </c>
-      <c r="T46" s="34"/>
-      <c r="U46" s="74">
+      <c r="T46" s="34">
+        <v>1</v>
+      </c>
+      <c r="V46" s="34"/>
+      <c r="W46" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V46" s="14"/>
-      <c r="Y46" s="6"/>
-    </row>
-    <row r="47" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="X46" s="14"/>
+      <c r="AA46" s="6"/>
+    </row>
+    <row r="47" spans="1:32" s="6" customFormat="1">
       <c r="A47" s="28"/>
       <c r="B47" s="29" t="s">
         <v>157</v>
@@ -4354,22 +4527,26 @@
       </c>
       <c r="R47" s="34"/>
       <c r="S47" s="34"/>
-      <c r="T47" s="34"/>
-      <c r="U47" s="74">
+      <c r="T47" s="34">
+        <v>1</v>
+      </c>
+      <c r="U47" s="34"/>
+      <c r="V47" s="34"/>
+      <c r="W47" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V47" s="14"/>
-      <c r="W47" s="3"/>
-      <c r="X47"/>
-      <c r="Y47"/>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="3"/>
       <c r="Z47"/>
       <c r="AA47"/>
       <c r="AB47"/>
       <c r="AC47"/>
       <c r="AD47"/>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE47"/>
+      <c r="AF47"/>
+    </row>
+    <row r="48" spans="1:32">
       <c r="A48" s="28"/>
       <c r="B48" s="29" t="s">
         <v>158</v>
@@ -4411,14 +4588,17 @@
       <c r="Q48" s="34">
         <v>1</v>
       </c>
-      <c r="T48" s="34"/>
-      <c r="U48" s="74">
+      <c r="T48" s="34">
+        <v>1</v>
+      </c>
+      <c r="V48" s="34"/>
+      <c r="W48" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V48" s="14"/>
-    </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X48" s="14"/>
+    </row>
+    <row r="49" spans="1:32">
       <c r="A49" s="28"/>
       <c r="B49" s="29" t="s">
         <v>159</v>
@@ -4460,14 +4640,17 @@
       <c r="Q49" s="34">
         <v>1</v>
       </c>
-      <c r="T49" s="34"/>
-      <c r="U49" s="74">
+      <c r="T49" s="34">
+        <v>1</v>
+      </c>
+      <c r="V49" s="34"/>
+      <c r="W49" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V49" s="14"/>
-    </row>
-    <row r="50" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X49" s="14"/>
+    </row>
+    <row r="50" spans="1:32" s="6" customFormat="1">
       <c r="A50" s="10"/>
       <c r="B50" s="22" t="s">
         <v>160</v>
@@ -4512,23 +4695,31 @@
         <v>0.5</v>
       </c>
       <c r="R50" s="34"/>
-      <c r="S50" s="34"/>
-      <c r="T50" s="32">
-        <v>1</v>
-      </c>
-      <c r="U50" s="83">
+      <c r="S50" s="34">
+        <v>1</v>
+      </c>
+      <c r="T50" s="34">
+        <v>1</v>
+      </c>
+      <c r="U50" s="34">
+        <v>1</v>
+      </c>
+      <c r="V50" s="32">
+        <v>1</v>
+      </c>
+      <c r="W50" s="72">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="V50" s="14"/>
-      <c r="W50" s="14"/>
-      <c r="Z50"/>
-      <c r="AA50"/>
+        <v>3</v>
+      </c>
+      <c r="X50" s="14"/>
+      <c r="Y50" s="14"/>
       <c r="AB50"/>
       <c r="AC50"/>
       <c r="AD50"/>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE50"/>
+      <c r="AF50"/>
+    </row>
+    <row r="51" spans="1:32">
       <c r="A51" s="11" t="s">
         <v>115</v>
       </c>
@@ -4572,18 +4763,22 @@
       <c r="Q51" s="33"/>
       <c r="R51" s="33"/>
       <c r="S51" s="33"/>
-      <c r="T51" s="33"/>
-      <c r="U51" s="74">
+      <c r="T51" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="U51" s="33"/>
+      <c r="V51" s="33"/>
+      <c r="W51" s="72">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V51" s="14"/>
-      <c r="AA51" s="31"/>
-      <c r="AB51" s="6"/>
-      <c r="AC51" s="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="X51" s="14"/>
+      <c r="AC51" s="31"/>
       <c r="AD51" s="6"/>
-    </row>
-    <row r="52" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE51" s="6"/>
+      <c r="AF51" s="6"/>
+    </row>
+    <row r="52" spans="1:32" s="6" customFormat="1">
       <c r="A52" s="10"/>
       <c r="B52" s="22" t="s">
         <v>162</v>
@@ -4631,22 +4826,26 @@
         <v>1</v>
       </c>
       <c r="S52" s="34"/>
-      <c r="T52" s="32"/>
-      <c r="U52" s="74">
+      <c r="T52" s="34">
+        <v>1</v>
+      </c>
+      <c r="U52" s="34"/>
+      <c r="V52" s="32"/>
+      <c r="W52" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V52" s="14"/>
-      <c r="W52" s="3"/>
-      <c r="X52"/>
-      <c r="Y52"/>
+        <v>1</v>
+      </c>
+      <c r="X52" s="14"/>
+      <c r="Y52" s="3"/>
       <c r="Z52"/>
-      <c r="AA52" s="31"/>
+      <c r="AA52"/>
       <c r="AB52"/>
-      <c r="AC52"/>
+      <c r="AC52" s="31"/>
       <c r="AD52"/>
-    </row>
-    <row r="53" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE52"/>
+      <c r="AF52"/>
+    </row>
+    <row r="53" spans="1:32" s="6" customFormat="1">
       <c r="A53" s="10"/>
       <c r="B53" s="22" t="s">
         <v>193</v>
@@ -4676,22 +4875,24 @@
       <c r="Q53" s="34"/>
       <c r="R53" s="34"/>
       <c r="S53" s="34"/>
-      <c r="T53" s="32"/>
-      <c r="U53" s="74">
+      <c r="T53" s="34"/>
+      <c r="U53" s="34"/>
+      <c r="V53" s="32"/>
+      <c r="W53" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V53" s="14"/>
-      <c r="W53" s="3"/>
-      <c r="X53" s="31"/>
-      <c r="Y53" s="31"/>
+      <c r="X53" s="14"/>
+      <c r="Y53" s="3"/>
       <c r="Z53" s="31"/>
       <c r="AA53" s="31"/>
       <c r="AB53" s="31"/>
       <c r="AC53" s="31"/>
       <c r="AD53" s="31"/>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE53" s="31"/>
+      <c r="AF53" s="31"/>
+    </row>
+    <row r="54" spans="1:32">
       <c r="B54" s="22" t="s">
         <v>189</v>
       </c>
@@ -4710,15 +4911,21 @@
       <c r="R54" s="34">
         <v>1</v>
       </c>
-      <c r="T54" s="32"/>
-      <c r="U54" s="74">
+      <c r="S54" s="34">
+        <v>1</v>
+      </c>
+      <c r="U54" s="34">
+        <v>1</v>
+      </c>
+      <c r="V54" s="32"/>
+      <c r="W54" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V54" s="14"/>
-      <c r="AA54" s="31"/>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X54" s="14"/>
+      <c r="AC54" s="31"/>
+    </row>
+    <row r="55" spans="1:32">
       <c r="B55" s="22" t="s">
         <v>163</v>
       </c>
@@ -4762,15 +4969,18 @@
       <c r="R55" s="34">
         <v>1</v>
       </c>
-      <c r="T55" s="32"/>
-      <c r="U55" s="74">
+      <c r="T55" s="34">
+        <v>1</v>
+      </c>
+      <c r="V55" s="32"/>
+      <c r="W55" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V55" s="14"/>
-      <c r="AA55" s="31"/>
-    </row>
-    <row r="56" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="X55" s="14"/>
+      <c r="AC55" s="31"/>
+    </row>
+    <row r="56" spans="1:32" s="31" customFormat="1">
       <c r="A56" s="10"/>
       <c r="B56" s="22" t="s">
         <v>164</v>
@@ -4800,15 +5010,17 @@
       <c r="Q56" s="34"/>
       <c r="R56" s="34"/>
       <c r="S56" s="34"/>
-      <c r="T56" s="32"/>
-      <c r="U56" s="74">
+      <c r="T56" s="34"/>
+      <c r="U56" s="34"/>
+      <c r="V56" s="32"/>
+      <c r="W56" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V56" s="14"/>
-      <c r="W56" s="3"/>
-    </row>
-    <row r="57" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X56" s="14"/>
+      <c r="Y56" s="3"/>
+    </row>
+    <row r="57" spans="1:32" s="31" customFormat="1">
       <c r="A57" s="10"/>
       <c r="B57" s="22" t="s">
         <v>165</v>
@@ -4836,15 +5048,17 @@
         <v>1</v>
       </c>
       <c r="S57" s="34"/>
-      <c r="T57" s="32"/>
-      <c r="U57" s="74">
+      <c r="T57" s="34"/>
+      <c r="U57" s="34"/>
+      <c r="V57" s="32"/>
+      <c r="W57" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V57" s="14"/>
-      <c r="W57" s="3"/>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="X57" s="14"/>
+      <c r="Y57" s="3"/>
+    </row>
+    <row r="58" spans="1:32">
       <c r="B58" s="22" t="s">
         <v>183</v>
       </c>
@@ -4872,16 +5086,19 @@
       <c r="R58" s="34">
         <v>1</v>
       </c>
-      <c r="T58" s="32"/>
-      <c r="U58" s="74">
+      <c r="T58" s="34">
+        <v>1</v>
+      </c>
+      <c r="V58" s="32"/>
+      <c r="W58" s="72">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="V58" s="14"/>
-      <c r="Y58" s="6"/>
-      <c r="AA58" s="31"/>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="X58" s="14"/>
+      <c r="AA58" s="6"/>
+      <c r="AC58" s="31"/>
+    </row>
+    <row r="59" spans="1:32">
       <c r="B59" s="22" t="s">
         <v>166</v>
       </c>
@@ -4907,15 +5124,18 @@
       <c r="P59" s="34">
         <v>1</v>
       </c>
-      <c r="T59" s="32"/>
-      <c r="U59" s="74">
+      <c r="T59" s="34">
+        <v>1</v>
+      </c>
+      <c r="V59" s="32"/>
+      <c r="W59" s="72">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V59" s="14"/>
-      <c r="AA59" s="31"/>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="X59" s="14"/>
+      <c r="AC59" s="31"/>
+    </row>
+    <row r="60" spans="1:32">
       <c r="B60" s="22" t="s">
         <v>167</v>
       </c>
@@ -4959,16 +5179,19 @@
       <c r="R60" s="34">
         <v>1</v>
       </c>
-      <c r="T60" s="32"/>
-      <c r="U60" s="83">
+      <c r="T60" s="34">
+        <v>1</v>
+      </c>
+      <c r="V60" s="32"/>
+      <c r="W60" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V60" s="14"/>
-      <c r="Z60" s="6"/>
-      <c r="AA60" s="31"/>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="X60" s="14"/>
+      <c r="AB60" s="6"/>
+      <c r="AC60" s="31"/>
+    </row>
+    <row r="61" spans="1:32">
       <c r="A61" s="11" t="s">
         <v>114</v>
       </c>
@@ -5012,15 +5235,19 @@
       </c>
       <c r="R61" s="33"/>
       <c r="S61" s="33"/>
-      <c r="T61" s="33"/>
-      <c r="U61" s="74">
+      <c r="T61" s="33">
+        <v>1</v>
+      </c>
+      <c r="U61" s="33"/>
+      <c r="V61" s="33"/>
+      <c r="W61" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V61" s="14"/>
-      <c r="AA61" s="31"/>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X61" s="14"/>
+      <c r="AC61" s="31"/>
+    </row>
+    <row r="62" spans="1:32">
       <c r="B62" s="22" t="s">
         <v>169</v>
       </c>
@@ -5064,18 +5291,21 @@
       <c r="R62" s="34">
         <v>1</v>
       </c>
-      <c r="T62" s="32"/>
-      <c r="U62" s="74">
+      <c r="T62" s="34">
+        <v>1</v>
+      </c>
+      <c r="V62" s="32"/>
+      <c r="W62" s="72">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V62" s="14"/>
-      <c r="AA62" s="31"/>
-      <c r="AB62" s="6"/>
-      <c r="AC62" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="X62" s="14"/>
+      <c r="AC62" s="31"/>
       <c r="AD62" s="6"/>
-    </row>
-    <row r="63" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE62" s="6"/>
+      <c r="AF62" s="6"/>
+    </row>
+    <row r="63" spans="1:32" s="31" customFormat="1">
       <c r="A63" s="10"/>
       <c r="B63" s="22" t="s">
         <v>206</v>
@@ -5103,18 +5333,22 @@
       </c>
       <c r="R63" s="34"/>
       <c r="S63" s="34"/>
-      <c r="T63" s="32"/>
-      <c r="U63" s="74">
+      <c r="T63" s="34">
+        <v>0.75</v>
+      </c>
+      <c r="U63" s="34"/>
+      <c r="V63" s="32"/>
+      <c r="W63" s="72">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V63" s="14"/>
-      <c r="W63" s="3"/>
-      <c r="AB63" s="6"/>
-      <c r="AC63" s="6"/>
+        <v>0.75</v>
+      </c>
+      <c r="X63" s="14"/>
+      <c r="Y63" s="3"/>
       <c r="AD63" s="6"/>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE63" s="6"/>
+      <c r="AF63" s="6"/>
+    </row>
+    <row r="64" spans="1:32">
       <c r="B64" s="22" t="s">
         <v>170</v>
       </c>
@@ -5155,15 +5389,18 @@
       <c r="R64" s="34">
         <v>1</v>
       </c>
-      <c r="T64" s="32"/>
-      <c r="U64" s="74">
+      <c r="T64" s="34">
+        <v>1</v>
+      </c>
+      <c r="V64" s="32"/>
+      <c r="W64" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="V64" s="14"/>
-      <c r="AA64" s="31"/>
-    </row>
-    <row r="65" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X64" s="14"/>
+      <c r="AC64" s="31"/>
+    </row>
+    <row r="65" spans="1:32" s="31" customFormat="1">
       <c r="A65" s="10"/>
       <c r="B65" s="22" t="s">
         <v>195</v>
@@ -5193,15 +5430,19 @@
       <c r="Q65" s="34"/>
       <c r="R65" s="34"/>
       <c r="S65" s="34"/>
-      <c r="T65" s="32"/>
-      <c r="U65" s="74">
+      <c r="T65" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="U65" s="34"/>
+      <c r="V65" s="32"/>
+      <c r="W65" s="72">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V65" s="14"/>
-      <c r="W65" s="3"/>
-    </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="X65" s="14"/>
+      <c r="Y65" s="3"/>
+    </row>
+    <row r="66" spans="1:32">
       <c r="B66" s="22" t="s">
         <v>171</v>
       </c>
@@ -5212,16 +5453,16 @@
       <c r="N66" s="34">
         <v>0</v>
       </c>
-      <c r="T66" s="32"/>
-      <c r="U66" s="83">
+      <c r="V66" s="32"/>
+      <c r="W66" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V66" s="14"/>
-      <c r="Z66" s="6"/>
-      <c r="AA66" s="31"/>
-    </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X66" s="14"/>
+      <c r="AB66" s="6"/>
+      <c r="AC66" s="31"/>
+    </row>
+    <row r="67" spans="1:32">
       <c r="A67" s="11" t="s">
         <v>113</v>
       </c>
@@ -5258,14 +5499,16 @@
       <c r="R67" s="33"/>
       <c r="S67" s="33"/>
       <c r="T67" s="33"/>
-      <c r="U67" s="74">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="V67" s="14"/>
-      <c r="AA67" s="31"/>
-    </row>
-    <row r="68" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U67" s="33"/>
+      <c r="V67" s="33"/>
+      <c r="W67" s="72">
+        <f t="shared" ref="W67:W81" si="4">SUM(T67:V67)</f>
+        <v>0</v>
+      </c>
+      <c r="X67" s="14"/>
+      <c r="AC67" s="31"/>
+    </row>
+    <row r="68" spans="1:32" s="31" customFormat="1">
       <c r="A68" s="28"/>
       <c r="B68" s="29" t="s">
         <v>196</v>
@@ -5297,17 +5540,19 @@
       </c>
       <c r="R68" s="34"/>
       <c r="S68" s="34"/>
-      <c r="T68" s="34">
-        <v>1</v>
-      </c>
-      <c r="U68" s="74">
-        <f t="shared" ref="U68:U81" si="2">SUM(Q68:T68)</f>
-        <v>1.5</v>
-      </c>
-      <c r="V68" s="14"/>
-      <c r="W68" s="3"/>
-    </row>
-    <row r="69" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T68" s="34"/>
+      <c r="U68" s="34"/>
+      <c r="V68" s="34">
+        <v>1</v>
+      </c>
+      <c r="W68" s="72">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="X68" s="14"/>
+      <c r="Y68" s="3"/>
+    </row>
+    <row r="69" spans="1:32" s="31" customFormat="1">
       <c r="A69" s="28"/>
       <c r="B69" s="29" t="s">
         <v>197</v>
@@ -5336,14 +5581,16 @@
       <c r="R69" s="34"/>
       <c r="S69" s="34"/>
       <c r="T69" s="34"/>
-      <c r="U69" s="74">
-        <f t="shared" si="2"/>
+      <c r="U69" s="34"/>
+      <c r="V69" s="34"/>
+      <c r="W69" s="72">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V69" s="14"/>
-      <c r="W69" s="3"/>
-    </row>
-    <row r="70" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X69" s="14"/>
+      <c r="Y69" s="3"/>
+    </row>
+    <row r="70" spans="1:32" s="31" customFormat="1">
       <c r="A70" s="28"/>
       <c r="B70" s="29" t="s">
         <v>198</v>
@@ -5372,14 +5619,16 @@
       <c r="R70" s="34"/>
       <c r="S70" s="34"/>
       <c r="T70" s="34"/>
-      <c r="U70" s="74">
-        <f t="shared" si="2"/>
+      <c r="U70" s="34"/>
+      <c r="V70" s="34"/>
+      <c r="W70" s="72">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V70" s="14"/>
-      <c r="W70" s="3"/>
-    </row>
-    <row r="71" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X70" s="14"/>
+      <c r="Y70" s="3"/>
+    </row>
+    <row r="71" spans="1:32" s="31" customFormat="1">
       <c r="A71" s="28"/>
       <c r="B71" s="29" t="s">
         <v>199</v>
@@ -5410,14 +5659,16 @@
       <c r="R71" s="34"/>
       <c r="S71" s="34"/>
       <c r="T71" s="34"/>
-      <c r="U71" s="74">
-        <f t="shared" si="2"/>
+      <c r="U71" s="34"/>
+      <c r="V71" s="34"/>
+      <c r="W71" s="72">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V71" s="14"/>
-      <c r="W71" s="3"/>
-    </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X71" s="14"/>
+      <c r="Y71" s="3"/>
+    </row>
+    <row r="72" spans="1:32">
       <c r="B72" s="22" t="s">
         <v>173</v>
       </c>
@@ -5440,14 +5691,14 @@
       <c r="Q72" s="34">
         <v>1</v>
       </c>
-      <c r="T72" s="32"/>
-      <c r="U72" s="83">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V72" s="14"/>
-    </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="V72" s="32"/>
+      <c r="W72" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X72" s="14"/>
+    </row>
+    <row r="73" spans="1:32">
       <c r="A73" s="11" t="s">
         <v>74</v>
       </c>
@@ -5490,13 +5741,15 @@
       <c r="R73" s="33"/>
       <c r="S73" s="33"/>
       <c r="T73" s="33"/>
-      <c r="U73" s="74">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V73" s="14"/>
-    </row>
-    <row r="74" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U73" s="33"/>
+      <c r="V73" s="33"/>
+      <c r="W73" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X73" s="14"/>
+    </row>
+    <row r="74" spans="1:32" s="6" customFormat="1">
       <c r="A74" s="28"/>
       <c r="B74" s="29" t="s">
         <v>82</v>
@@ -5537,21 +5790,23 @@
       <c r="R74" s="34"/>
       <c r="S74" s="34"/>
       <c r="T74" s="34"/>
-      <c r="U74" s="74">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V74" s="14"/>
-      <c r="W74" s="3"/>
-      <c r="X74"/>
-      <c r="Y74"/>
+      <c r="U74" s="34"/>
+      <c r="V74" s="34"/>
+      <c r="W74" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X74" s="14"/>
+      <c r="Y74" s="3"/>
       <c r="Z74"/>
       <c r="AA74"/>
       <c r="AB74"/>
       <c r="AC74"/>
       <c r="AD74"/>
-    </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE74"/>
+      <c r="AF74"/>
+    </row>
+    <row r="75" spans="1:32">
       <c r="B75" s="22" t="s">
         <v>93</v>
       </c>
@@ -5564,16 +5819,16 @@
       <c r="I75" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="T75" s="32"/>
-      <c r="U75" s="74">
-        <f t="shared" si="2"/>
+      <c r="V75" s="32"/>
+      <c r="W75" s="72">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V75" s="14"/>
-      <c r="X75" s="31"/>
-      <c r="Z75" s="6"/>
-    </row>
-    <row r="76" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X75" s="14"/>
+      <c r="Z75" s="31"/>
+      <c r="AB75" s="6"/>
+    </row>
+    <row r="76" spans="1:32" s="31" customFormat="1">
       <c r="A76" s="10"/>
       <c r="B76" s="22" t="s">
         <v>94</v>
@@ -5613,16 +5868,18 @@
       </c>
       <c r="R76" s="34"/>
       <c r="S76" s="34"/>
-      <c r="T76" s="32"/>
-      <c r="U76" s="74">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V76" s="14"/>
-      <c r="W76" s="3"/>
-      <c r="Z76" s="6"/>
-    </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="T76" s="34"/>
+      <c r="U76" s="34"/>
+      <c r="V76" s="32"/>
+      <c r="W76" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X76" s="14"/>
+      <c r="Y76" s="3"/>
+      <c r="AB76" s="6"/>
+    </row>
+    <row r="77" spans="1:32">
       <c r="B77" s="22" t="s">
         <v>177</v>
       </c>
@@ -5636,18 +5893,18 @@
       <c r="N77" s="34">
         <v>1</v>
       </c>
-      <c r="T77" s="32"/>
-      <c r="U77" s="74">
-        <f t="shared" si="2"/>
+      <c r="V77" s="32"/>
+      <c r="W77" s="72">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V77" s="14"/>
-      <c r="AA77" s="6"/>
-      <c r="AB77" s="6"/>
+      <c r="X77" s="14"/>
       <c r="AC77" s="6"/>
       <c r="AD77" s="6"/>
-    </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE77" s="6"/>
+      <c r="AF77" s="6"/>
+    </row>
+    <row r="78" spans="1:32">
       <c r="B78" s="22" t="s">
         <v>95</v>
       </c>
@@ -5681,14 +5938,14 @@
       <c r="Q78" s="34">
         <v>1</v>
       </c>
-      <c r="T78" s="32"/>
-      <c r="U78" s="74">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V78" s="14"/>
-    </row>
-    <row r="79" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V78" s="32"/>
+      <c r="W78" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X78" s="14"/>
+    </row>
+    <row r="79" spans="1:32" s="6" customFormat="1">
       <c r="A79" s="10"/>
       <c r="B79" s="22" t="s">
         <v>96</v>
@@ -5728,22 +5985,24 @@
       </c>
       <c r="R79" s="34"/>
       <c r="S79" s="34"/>
-      <c r="T79" s="32"/>
-      <c r="U79" s="74">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V79" s="14"/>
-      <c r="W79" s="3"/>
-      <c r="X79"/>
-      <c r="Y79"/>
+      <c r="T79" s="34"/>
+      <c r="U79" s="34"/>
+      <c r="V79" s="32"/>
+      <c r="W79" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X79" s="14"/>
+      <c r="Y79" s="3"/>
       <c r="Z79"/>
       <c r="AA79"/>
       <c r="AB79"/>
       <c r="AC79"/>
       <c r="AD79"/>
-    </row>
-    <row r="80" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AE79"/>
+      <c r="AF79"/>
+    </row>
+    <row r="80" spans="1:32" s="6" customFormat="1">
       <c r="A80" s="10"/>
       <c r="B80" s="22" t="s">
         <v>208</v>
@@ -5773,22 +6032,24 @@
       </c>
       <c r="R80" s="34"/>
       <c r="S80" s="34"/>
-      <c r="T80" s="32"/>
-      <c r="U80" s="74">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="V80" s="14"/>
-      <c r="W80" s="3"/>
-      <c r="X80" s="31"/>
-      <c r="Y80" s="31"/>
+      <c r="T80" s="34"/>
+      <c r="U80" s="34"/>
+      <c r="V80" s="32"/>
+      <c r="W80" s="72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X80" s="14"/>
+      <c r="Y80" s="3"/>
       <c r="Z80" s="31"/>
       <c r="AA80" s="31"/>
       <c r="AB80" s="31"/>
       <c r="AC80" s="31"/>
       <c r="AD80" s="31"/>
-    </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE80" s="31"/>
+      <c r="AF80" s="31"/>
+    </row>
+    <row r="81" spans="1:32">
       <c r="B81" s="23" t="s">
         <v>97</v>
       </c>
@@ -5824,22 +6085,24 @@
       <c r="R81" s="35"/>
       <c r="S81" s="35"/>
       <c r="T81" s="35"/>
-      <c r="U81" s="83">
-        <f t="shared" si="2"/>
+      <c r="U81" s="35"/>
+      <c r="V81" s="35"/>
+      <c r="W81" s="72">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V81" s="14"/>
-    </row>
-    <row r="82" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="X81" s="14"/>
+    </row>
+    <row r="82" spans="1:32" ht="15" thickBot="1">
       <c r="A82" s="11"/>
-      <c r="V82" s="14"/>
-      <c r="Y82" s="31"/>
-    </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X82" s="14"/>
+      <c r="AA82" s="31"/>
+    </row>
+    <row r="83" spans="1:32">
       <c r="I83" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="J83" s="80"/>
+      <c r="J83" s="78"/>
       <c r="K83" s="62"/>
       <c r="L83" s="62"/>
       <c r="M83" s="62"/>
@@ -5847,26 +6110,28 @@
       <c r="O83" s="62"/>
       <c r="P83" s="62"/>
       <c r="Q83" s="62">
-        <f t="array" ref="Q83">SUM($C2:$C81*(Q2:Q81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>197</v>
+        <f t="array" ref="Q83">SUM($C2:$C81*(Q2:Q81&gt;=0.9)*($W2:$W81&gt;=$Y$12))</f>
+        <v>148</v>
       </c>
       <c r="R83" s="62">
-        <f t="array" ref="R83">SUM($C2:$C81*(R2:R81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>126</v>
+        <f t="array" ref="R83">SUM($C2:$C81*(R2:R81&gt;=0.9)*($W2:$W81&gt;=$Y$12))</f>
+        <v>104</v>
       </c>
       <c r="S83" s="62"/>
-      <c r="T83" s="63"/>
-      <c r="V83" s="14"/>
-      <c r="AA83" s="6"/>
-      <c r="AB83" s="6"/>
+      <c r="T83" s="62"/>
+      <c r="U83" s="62"/>
+      <c r="V83" s="63"/>
+      <c r="X83" s="14"/>
       <c r="AC83" s="6"/>
       <c r="AD83" s="6"/>
-    </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE83" s="6"/>
+      <c r="AF83" s="6"/>
+    </row>
+    <row r="84" spans="1:32">
       <c r="I84" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="J84" s="81"/>
+      <c r="J84" s="79"/>
       <c r="K84" s="65"/>
       <c r="L84" s="65"/>
       <c r="M84" s="65"/>
@@ -5874,18 +6139,20 @@
       <c r="O84" s="65"/>
       <c r="P84" s="65"/>
       <c r="Q84" s="65">
-        <f t="array" ref="Q84">SUM($C2:$C81*Q2:Q81*($U2:$U81&gt;=$W$12))</f>
-        <v>202.5</v>
+        <f t="array" ref="Q84">SUM($C2:$C81*Q2:Q81*($W2:$W81&gt;=$Y$12))</f>
+        <v>153.5</v>
       </c>
       <c r="R84" s="65">
-        <f t="array" ref="R84">SUM($C2:$C81*R2:R81*($U2:$U81&gt;=$W$12))</f>
-        <v>126</v>
+        <f t="array" ref="R84">SUM($C2:$C81*R2:R81*($W2:$W81&gt;=$Y$12))</f>
+        <v>104</v>
       </c>
       <c r="S84" s="65"/>
-      <c r="T84" s="66"/>
-      <c r="V84" s="14"/>
-    </row>
-    <row r="85" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T84" s="65"/>
+      <c r="U84" s="65"/>
+      <c r="V84" s="66"/>
+      <c r="X84" s="14"/>
+    </row>
+    <row r="85" spans="1:32" s="6" customFormat="1">
       <c r="A85" s="10"/>
       <c r="B85" s="22"/>
       <c r="C85" s="13"/>
@@ -5897,7 +6164,7 @@
       <c r="I85" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="J85" s="81"/>
+      <c r="J85" s="79"/>
       <c r="K85" s="65"/>
       <c r="L85" s="65"/>
       <c r="M85" s="65"/>
@@ -5905,31 +6172,33 @@
       <c r="O85" s="65"/>
       <c r="P85" s="65"/>
       <c r="Q85" s="65">
-        <f t="array" ref="Q85">SUM($C$2:$C$81*(Q$2:Q$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>208</v>
+        <f t="array" ref="Q85">SUM($C$2:$C$81*(Q$2:Q$81&gt;=0.1)*($W$2:$W$81&gt;=$Y$12))</f>
+        <v>159</v>
       </c>
       <c r="R85" s="65">
-        <f t="array" ref="R85">SUM($C$2:$C$81*(R$2:R$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>126</v>
+        <f t="array" ref="R85">SUM($C$2:$C$81*(R$2:R$81&gt;=0.1)*($W$2:$W$81&gt;=$Y$12))</f>
+        <v>104</v>
       </c>
       <c r="S85" s="65"/>
-      <c r="T85" s="66"/>
-      <c r="U85" s="3"/>
-      <c r="V85" s="14"/>
+      <c r="T85" s="65"/>
+      <c r="U85" s="65"/>
+      <c r="V85" s="66"/>
       <c r="W85" s="3"/>
-      <c r="X85"/>
-      <c r="Y85"/>
+      <c r="X85" s="14"/>
+      <c r="Y85" s="3"/>
       <c r="Z85"/>
       <c r="AA85"/>
       <c r="AB85"/>
       <c r="AC85"/>
       <c r="AD85"/>
-    </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE85"/>
+      <c r="AF85"/>
+    </row>
+    <row r="86" spans="1:32">
       <c r="I86" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="J86" s="81"/>
+      <c r="J86" s="79"/>
       <c r="K86" s="65"/>
       <c r="L86" s="65"/>
       <c r="M86" s="65"/>
@@ -5937,26 +6206,28 @@
       <c r="O86" s="65"/>
       <c r="P86" s="65"/>
       <c r="Q86" s="65">
-        <f t="shared" ref="Q86:R86" si="3">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
-        <v>236</v>
+        <f t="shared" ref="Q86:R86" si="5">LOOKUP($Y$12,$Y23:$Y31,$Z23:$Z31)</f>
+        <v>180</v>
       </c>
       <c r="R86" s="65">
-        <f t="shared" si="3"/>
-        <v>236</v>
+        <f t="shared" si="5"/>
+        <v>180</v>
       </c>
       <c r="S86" s="65"/>
-      <c r="T86" s="66"/>
-      <c r="V86" s="14"/>
-      <c r="AA86" s="6"/>
-      <c r="AB86" s="6"/>
+      <c r="T86" s="65"/>
+      <c r="U86" s="65"/>
+      <c r="V86" s="66"/>
+      <c r="X86" s="14"/>
       <c r="AC86" s="6"/>
       <c r="AD86" s="6"/>
-    </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE86" s="6"/>
+      <c r="AF86" s="6"/>
+    </row>
+    <row r="87" spans="1:32">
       <c r="I87" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="J87" s="81"/>
+      <c r="J87" s="79"/>
       <c r="K87" s="67"/>
       <c r="L87" s="67"/>
       <c r="M87" s="67"/>
@@ -5964,23 +6235,25 @@
       <c r="O87" s="67"/>
       <c r="P87" s="67"/>
       <c r="Q87" s="67">
-        <f t="shared" ref="Q87:R87" si="4">Q84/Q86</f>
-        <v>0.85805084745762716</v>
+        <f t="shared" ref="Q87:R87" si="6">Q84/Q86</f>
+        <v>0.85277777777777775</v>
       </c>
       <c r="R87" s="67">
-        <f t="shared" si="4"/>
-        <v>0.53389830508474578</v>
+        <f t="shared" si="6"/>
+        <v>0.57777777777777772</v>
       </c>
       <c r="S87" s="67"/>
-      <c r="T87" s="68"/>
-      <c r="V87" s="14"/>
-    </row>
-    <row r="88" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T87" s="67"/>
+      <c r="U87" s="67"/>
+      <c r="V87" s="68"/>
+      <c r="X87" s="14"/>
+    </row>
+    <row r="88" spans="1:32" ht="15" thickBot="1">
       <c r="C88" s="31"/>
       <c r="I88" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="J88" s="82"/>
+      <c r="J88" s="80"/>
       <c r="K88" s="70"/>
       <c r="L88" s="70"/>
       <c r="M88" s="70"/>
@@ -5988,74 +6261,76 @@
       <c r="O88" s="70"/>
       <c r="P88" s="70"/>
       <c r="Q88" s="70">
-        <f t="shared" ref="Q88:R88" si="5">Q86-Q84</f>
-        <v>33.5</v>
+        <f t="shared" ref="Q88:R88" si="7">Q86-Q84</f>
+        <v>26.5</v>
       </c>
       <c r="R88" s="70">
-        <f t="shared" si="5"/>
-        <v>110</v>
+        <f t="shared" si="7"/>
+        <v>76</v>
       </c>
       <c r="S88" s="70"/>
-      <c r="T88" s="71"/>
-      <c r="V88" s="14"/>
-      <c r="AA88" s="6"/>
-      <c r="AB88" s="6"/>
+      <c r="T88" s="70"/>
+      <c r="U88" s="70"/>
+      <c r="V88" s="71"/>
+      <c r="X88" s="14"/>
       <c r="AC88" s="6"/>
       <c r="AD88" s="6"/>
-    </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE88" s="6"/>
+      <c r="AF88" s="6"/>
+    </row>
+    <row r="89" spans="1:32">
       <c r="C89" s="31"/>
-      <c r="V89" s="14"/>
-    </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X89" s="14"/>
+    </row>
+    <row r="90" spans="1:32">
       <c r="C90" s="31"/>
       <c r="I90" s="13"/>
       <c r="J90" s="13"/>
       <c r="K90" s="13"/>
-      <c r="V90" s="14"/>
-    </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X90" s="14"/>
+    </row>
+    <row r="91" spans="1:32">
       <c r="C91" s="31"/>
       <c r="I91" s="13"/>
       <c r="J91" s="13"/>
       <c r="K91" s="13"/>
-      <c r="V91" s="14"/>
-    </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X91" s="14"/>
+    </row>
+    <row r="92" spans="1:32">
       <c r="I92" s="13"/>
       <c r="J92" s="13"/>
       <c r="K92" s="13"/>
-      <c r="V92" s="14"/>
-    </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X92" s="14"/>
+    </row>
+    <row r="93" spans="1:32">
       <c r="I93" s="13"/>
       <c r="J93" s="13"/>
       <c r="K93" s="13"/>
-      <c r="V93" s="14"/>
-      <c r="Z93" s="31"/>
-    </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X93" s="14"/>
+      <c r="AB93" s="31"/>
+    </row>
+    <row r="94" spans="1:32">
       <c r="I94" s="13"/>
       <c r="J94" s="13"/>
       <c r="K94" s="13"/>
-      <c r="V94" s="14"/>
-    </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="X94" s="14"/>
+    </row>
+    <row r="95" spans="1:32">
       <c r="I95" s="13"/>
       <c r="J95" s="13"/>
       <c r="K95" s="13"/>
     </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:32">
       <c r="I96" s="13"/>
       <c r="J96" s="13"/>
       <c r="K96" s="13"/>
     </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:32">
       <c r="I97" s="13"/>
       <c r="J97" s="13"/>
       <c r="K97" s="13"/>
     </row>
-    <row r="98" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:32" s="31" customFormat="1">
       <c r="A98" s="10"/>
       <c r="B98" s="22"/>
       <c r="C98" s="13"/>
@@ -6075,57 +6350,64 @@
       <c r="Q98" s="34"/>
       <c r="R98" s="34"/>
       <c r="S98" s="34"/>
-      <c r="T98" s="2"/>
-      <c r="U98" s="3"/>
-      <c r="V98" s="3"/>
+      <c r="T98" s="34"/>
+      <c r="U98" s="34"/>
+      <c r="V98" s="2"/>
       <c r="W98" s="3"/>
-      <c r="X98"/>
-      <c r="Y98"/>
+      <c r="X98" s="3"/>
+      <c r="Y98" s="3"/>
       <c r="Z98"/>
       <c r="AA98"/>
       <c r="AB98"/>
       <c r="AC98"/>
       <c r="AD98"/>
-    </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA101" s="6"/>
-      <c r="AB101" s="6"/>
+      <c r="AE98"/>
+      <c r="AF98"/>
+    </row>
+    <row r="101" spans="1:32">
       <c r="AC101" s="6"/>
       <c r="AD101" s="6"/>
-    </row>
-    <row r="105" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA105" s="6"/>
-      <c r="AB105" s="6"/>
+      <c r="AE101" s="6"/>
+      <c r="AF101" s="6"/>
+    </row>
+    <row r="105" spans="1:32">
       <c r="AC105" s="6"/>
       <c r="AD105" s="6"/>
-    </row>
-    <row r="110" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="AA110" s="6"/>
-      <c r="AB110" s="6"/>
+      <c r="AE105" s="6"/>
+      <c r="AF105" s="6"/>
+    </row>
+    <row r="110" spans="1:32">
       <c r="AC110" s="6"/>
       <c r="AD110" s="6"/>
-    </row>
-    <row r="123" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA123" s="31"/>
-      <c r="AB123" s="31"/>
+      <c r="AE110" s="6"/>
+      <c r="AF110" s="6"/>
+    </row>
+    <row r="123" spans="29:32">
       <c r="AC123" s="31"/>
       <c r="AD123" s="31"/>
+      <c r="AE123" s="31"/>
+      <c r="AF123" s="31"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U81">
+  <conditionalFormatting sqref="B2:W81">
     <cfRule type="expression" dxfId="2" priority="43" stopIfTrue="1">
-      <formula>$U2&gt;=(0.5+$W$12)</formula>
+      <formula>$W2&gt;=(0.5+$Y$12)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="44" stopIfTrue="1">
-      <formula>$U2&gt;=$W$12</formula>
+      <formula>$W2&gt;=$Y$12</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="45">
-      <formula>$U2&gt;=($W$12-0.5)</formula>
+      <formula>$W2&gt;=($Y$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6137,377 +6419,382 @@
       <selection sqref="A1:A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1">
       <c r="A68" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes to master and spreadsheet for spring 2020
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2021spring.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2021spring.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20342"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\131\StudentGuideModule1\what_labs_to_include\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469701E0-A459-4E30-923A-D48095CB58CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4920" yWindow="0" windowWidth="30160" windowHeight="16120" tabRatio="539"/>
+    <workbookView xWindow="-4920" yWindow="0" windowWidth="30156" windowHeight="16116" tabRatio="539" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Matt Trawick</author>
   </authors>
   <commentList>
-    <comment ref="Y1" authorId="0">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -118,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z11" authorId="0">
+    <comment ref="X11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -171,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA19" authorId="0">
+    <comment ref="Y19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -196,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y22" authorId="0">
+    <comment ref="W22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -229,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z22" authorId="0">
+    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -253,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB22" authorId="0">
+    <comment ref="Z22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -278,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N61" authorId="0">
+    <comment ref="N61" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -307,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="210">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -914,9 +920,6 @@
     <t>added by Matt, 2019</t>
   </si>
   <si>
-    <t>2020 spr Mariama</t>
-  </si>
-  <si>
     <t>2020 spr Barti</t>
   </si>
   <si>
@@ -924,9 +927,6 @@
   </si>
   <si>
     <t>2020 fall Ovidiu</t>
-  </si>
-  <si>
-    <t>2020 fall Haw</t>
   </si>
   <si>
     <t>Derivatives of Sine and Cosine Functions</t>
@@ -950,9 +950,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1602,12 +1602,12 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1619,11 +1619,11 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="14" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1637,7 +1637,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1797,6 +1797,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2210,33 +2214,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF123"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="W50" sqref="W50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="13" customWidth="1"/>
-    <col min="4" max="8" width="5.83203125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="28.5" style="19" customWidth="1"/>
-    <col min="10" max="11" width="10.1640625" style="34" customWidth="1"/>
-    <col min="12" max="14" width="8.83203125" style="34" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" style="34" customWidth="1"/>
-    <col min="16" max="21" width="8.83203125" style="34" customWidth="1"/>
-    <col min="22" max="22" width="8.83203125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="11" style="3" customWidth="1"/>
-    <col min="24" max="24" width="2.5" style="3" customWidth="1"/>
-    <col min="25" max="25" width="10.33203125" style="3" customWidth="1"/>
-    <col min="27" max="27" width="9.5" customWidth="1"/>
-    <col min="28" max="28" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="13" customWidth="1"/>
+    <col min="4" max="8" width="5.77734375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="19" customWidth="1"/>
+    <col min="10" max="11" width="10.109375" style="34" customWidth="1"/>
+    <col min="12" max="19" width="8.77734375" style="34" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="11" style="3" customWidth="1"/>
+    <col min="22" max="22" width="2.44140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="9.44140625" customWidth="1"/>
+    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="1" customFormat="1" ht="28">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>73</v>
       </c>
@@ -2289,34 +2291,28 @@
         <v>203</v>
       </c>
       <c r="R1" s="47" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="S1" s="47" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="T1" s="47" t="s">
-        <v>210</v>
-      </c>
-      <c r="U1" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="V1" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="W1" s="50" t="s">
+      <c r="U1" s="50" t="s">
         <v>181</v>
       </c>
+      <c r="V1" s="30"/>
+      <c r="W1" s="31"/>
       <c r="X1" s="30"/>
-      <c r="Y1" s="31"/>
+      <c r="Y1" s="30"/>
       <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
       <c r="AC1" s="31"/>
       <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-    </row>
-    <row r="2" spans="1:32" s="1" customFormat="1">
+    </row>
+    <row r="2" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>86</v>
       </c>
@@ -2344,26 +2340,24 @@
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
       <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="53">
+      <c r="T2" s="53">
         <v>3</v>
       </c>
-      <c r="W2" s="72">
-        <f>SUM(T2:V2)</f>
+      <c r="U2" s="72">
+        <f>SUM(R2:T2)</f>
         <v>3</v>
       </c>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
       <c r="X2" s="73"/>
       <c r="Y2" s="73"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="30"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
       <c r="AC2" s="31"/>
       <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-    </row>
-    <row r="3" spans="1:32" s="1" customFormat="1">
+    </row>
+    <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="46"/>
       <c r="B3" s="52" t="s">
         <v>88</v>
@@ -2389,26 +2383,24 @@
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
       <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57"/>
-      <c r="V3" s="57">
+      <c r="T3" s="57">
         <v>3</v>
       </c>
-      <c r="W3" s="72">
-        <f t="shared" ref="W3:W66" si="0">SUM(T3:V3)</f>
+      <c r="U3" s="72">
+        <f t="shared" ref="U3:U66" si="0">SUM(R3:T3)</f>
         <v>3</v>
       </c>
+      <c r="V3" s="73"/>
+      <c r="W3" s="73"/>
       <c r="X3" s="73"/>
       <c r="Y3" s="73"/>
-      <c r="Z3" s="73"/>
-      <c r="AA3" s="73"/>
-      <c r="AB3" s="30"/>
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
       <c r="AC3" s="31"/>
       <c r="AD3" s="31"/>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="31"/>
-    </row>
-    <row r="4" spans="1:32" s="1" customFormat="1">
+    </row>
+    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>110</v>
       </c>
@@ -2442,34 +2434,30 @@
         <v>0.2</v>
       </c>
       <c r="O4" s="34">
+        <v>0</v>
+      </c>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34">
         <v>0.5</v>
       </c>
-      <c r="P4" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
       <c r="S4" s="34"/>
-      <c r="T4" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="72">
+      <c r="T4" s="33"/>
+      <c r="U4" s="81">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
       <c r="AC4" s="31"/>
       <c r="AD4" s="31"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="31"/>
-    </row>
-    <row r="5" spans="1:32">
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>120</v>
       </c>
@@ -2483,22 +2471,22 @@
       <c r="N5" s="34">
         <v>0</v>
       </c>
-      <c r="V5" s="32"/>
-      <c r="W5" s="72">
+      <c r="T5" s="32"/>
+      <c r="U5" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
       <c r="AC5" s="31"/>
       <c r="AD5" s="31"/>
-      <c r="AE5" s="31"/>
-      <c r="AF5" s="31"/>
-    </row>
-    <row r="6" spans="1:32">
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="28"/>
       <c r="B6" s="29" t="s">
         <v>121</v>
@@ -2510,22 +2498,22 @@
       <c r="N6" s="34">
         <v>0</v>
       </c>
-      <c r="V6" s="34"/>
-      <c r="W6" s="72">
+      <c r="T6" s="34"/>
+      <c r="U6" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="31"/>
+      <c r="AB6" s="31"/>
       <c r="AC6" s="31"/>
       <c r="AD6" s="31"/>
-      <c r="AE6" s="31"/>
-      <c r="AF6" s="31"/>
-    </row>
-    <row r="7" spans="1:32" s="31" customFormat="1">
+    </row>
+    <row r="7" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="22" t="s">
         <v>122</v>
@@ -2551,20 +2539,18 @@
       <c r="Q7" s="34"/>
       <c r="R7" s="34"/>
       <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="72">
+      <c r="T7" s="32"/>
+      <c r="U7" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="14"/>
-    </row>
-    <row r="8" spans="1:32">
+      <c r="Z7" s="14"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B8" s="22" t="s">
         <v>123</v>
       </c>
@@ -2575,22 +2561,22 @@
       <c r="N8" s="34">
         <v>0</v>
       </c>
-      <c r="V8" s="32"/>
-      <c r="W8" s="72">
+      <c r="T8" s="32"/>
+      <c r="U8" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
       <c r="AC8" s="31"/>
       <c r="AD8" s="31"/>
-      <c r="AE8" s="31"/>
-      <c r="AF8" s="31"/>
-    </row>
-    <row r="9" spans="1:32">
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
         <v>124</v>
       </c>
@@ -2637,28 +2623,22 @@
       <c r="S9" s="34">
         <v>1</v>
       </c>
-      <c r="T9" s="34">
-        <v>1</v>
-      </c>
-      <c r="U9" s="34">
-        <v>1</v>
-      </c>
-      <c r="V9" s="32"/>
-      <c r="W9" s="72">
+      <c r="T9" s="32"/>
+      <c r="U9" s="72">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="31"/>
+      <c r="AB9" s="31"/>
       <c r="AC9" s="31"/>
       <c r="AD9" s="31"/>
-      <c r="AE9" s="31"/>
-      <c r="AF9" s="31"/>
-    </row>
-    <row r="10" spans="1:32" ht="15" thickBot="1">
+    </row>
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="22" t="s">
         <v>125</v>
       </c>
@@ -2705,28 +2685,22 @@
       <c r="S10" s="34">
         <v>1</v>
       </c>
-      <c r="T10" s="34">
-        <v>1</v>
-      </c>
-      <c r="U10" s="34">
-        <v>1</v>
-      </c>
-      <c r="V10" s="32"/>
-      <c r="W10" s="72">
+      <c r="T10" s="32"/>
+      <c r="U10" s="72">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31"/>
       <c r="AC10" s="31"/>
       <c r="AD10" s="31"/>
-      <c r="AE10" s="31"/>
-      <c r="AF10" s="31"/>
-    </row>
-    <row r="11" spans="1:32">
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
         <v>126</v>
       </c>
@@ -2770,30 +2744,24 @@
       <c r="S11" s="34">
         <v>1</v>
       </c>
-      <c r="T11" s="34">
-        <v>1</v>
-      </c>
-      <c r="U11" s="34">
-        <v>1</v>
-      </c>
-      <c r="V11" s="32"/>
-      <c r="W11" s="72">
+      <c r="T11" s="32"/>
+      <c r="U11" s="72">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="40" t="s">
+      <c r="V11" s="5"/>
+      <c r="W11" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="14"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="31"/>
+      <c r="AB11" s="31"/>
       <c r="AC11" s="31"/>
       <c r="AD11" s="31"/>
-      <c r="AE11" s="31"/>
-      <c r="AF11" s="31"/>
-    </row>
-    <row r="12" spans="1:32" ht="15" thickBot="1">
+    </row>
+    <row r="12" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="22" t="s">
         <v>127</v>
       </c>
@@ -2804,24 +2772,24 @@
       <c r="N12" s="34">
         <v>0</v>
       </c>
-      <c r="V12" s="32"/>
-      <c r="W12" s="72">
+      <c r="T12" s="32"/>
+      <c r="U12" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="42">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="42">
+        <v>1</v>
+      </c>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="31"/>
       <c r="AC12" s="31"/>
       <c r="AD12" s="31"/>
-      <c r="AE12" s="31"/>
-      <c r="AF12" s="31"/>
-    </row>
-    <row r="13" spans="1:32">
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
         <v>175</v>
       </c>
@@ -2862,25 +2830,22 @@
       <c r="R13" s="34">
         <v>1</v>
       </c>
-      <c r="T13" s="34">
-        <v>1</v>
-      </c>
-      <c r="V13" s="32"/>
-      <c r="W13" s="72">
+      <c r="T13" s="32"/>
+      <c r="U13" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="31"/>
-      <c r="Z13" s="31"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="14"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="31"/>
+      <c r="AB13" s="31"/>
       <c r="AC13" s="31"/>
       <c r="AD13" s="31"/>
-      <c r="AE13" s="31"/>
-      <c r="AF13" s="31"/>
-    </row>
-    <row r="14" spans="1:32" ht="15" thickBot="1">
+    </row>
+    <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
         <v>128</v>
       </c>
@@ -2921,26 +2886,23 @@
       <c r="R14" s="34">
         <v>1</v>
       </c>
-      <c r="T14" s="34">
-        <v>1</v>
-      </c>
-      <c r="V14" s="32"/>
-      <c r="W14" s="72">
+      <c r="T14" s="32"/>
+      <c r="U14" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="1" t="s">
+      <c r="V14" s="5"/>
+      <c r="W14" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="14"/>
       <c r="AA14" s="31"/>
-      <c r="AB14" s="14"/>
+      <c r="AB14" s="31"/>
       <c r="AC14" s="31"/>
       <c r="AD14" s="31"/>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31"/>
-    </row>
-    <row r="15" spans="1:32">
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
         <v>174</v>
       </c>
@@ -2954,29 +2916,26 @@
       <c r="N15" s="34">
         <v>0</v>
       </c>
-      <c r="O15" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="V15" s="32"/>
-      <c r="W15" s="72">
+      <c r="T15" s="32"/>
+      <c r="U15" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="16" t="s">
+      <c r="V15" s="5"/>
+      <c r="W15" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="Z15" s="36"/>
-      <c r="AA15" s="15">
+      <c r="X15" s="36"/>
+      <c r="Y15" s="15">
         <v>0.05</v>
       </c>
+      <c r="Z15" s="31"/>
+      <c r="AA15" s="31"/>
       <c r="AB15" s="31"/>
       <c r="AC15" s="31"/>
       <c r="AD15" s="31"/>
-      <c r="AE15" s="31"/>
-      <c r="AF15" s="31"/>
-    </row>
-    <row r="16" spans="1:32">
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B16" s="22" t="s">
         <v>129</v>
       </c>
@@ -2990,29 +2949,26 @@
       <c r="N16" s="34">
         <v>0.01</v>
       </c>
-      <c r="O16" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="V16" s="32"/>
-      <c r="W16" s="72">
+      <c r="T16" s="32"/>
+      <c r="U16" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="V16" s="5"/>
+      <c r="W16" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="X16" s="5"/>
-      <c r="Y16" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z16" s="5"/>
-      <c r="AA16" s="8">
+      <c r="Y16" s="8">
         <v>0.3</v>
       </c>
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="31"/>
       <c r="AB16" s="31"/>
       <c r="AC16" s="31"/>
       <c r="AD16" s="31"/>
-      <c r="AE16" s="31"/>
-      <c r="AF16" s="31"/>
-    </row>
-    <row r="17" spans="1:32">
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B17" s="22" t="s">
         <v>130</v>
       </c>
@@ -3038,35 +2994,32 @@
       <c r="N17" s="34">
         <v>0.8</v>
       </c>
-      <c r="O17" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="34">
-        <v>1</v>
-      </c>
-      <c r="T17" s="34">
+      <c r="P17" s="34">
+        <v>1</v>
+      </c>
+      <c r="R17" s="34">
         <v>0.75</v>
       </c>
-      <c r="V17" s="32"/>
-      <c r="W17" s="72">
+      <c r="T17" s="32"/>
+      <c r="U17" s="72">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
+      <c r="V17" s="5"/>
+      <c r="W17" s="17" t="s">
+        <v>78</v>
+      </c>
       <c r="X17" s="5"/>
-      <c r="Y17" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="8">
+      <c r="Y17" s="8">
         <v>3</v>
       </c>
+      <c r="Z17" s="31"/>
+      <c r="AA17" s="31"/>
       <c r="AB17" s="31"/>
       <c r="AC17" s="31"/>
       <c r="AD17" s="31"/>
-      <c r="AE17" s="31"/>
-      <c r="AF17" s="31"/>
-    </row>
-    <row r="18" spans="1:32">
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B18" s="22" t="s">
         <v>131</v>
       </c>
@@ -3104,32 +3057,29 @@
       <c r="P18" s="34">
         <v>1</v>
       </c>
-      <c r="Q18" s="34">
-        <v>1</v>
-      </c>
-      <c r="T18" s="34">
-        <v>1</v>
-      </c>
-      <c r="V18" s="32"/>
-      <c r="W18" s="72">
+      <c r="R18" s="34">
+        <v>1</v>
+      </c>
+      <c r="T18" s="32"/>
+      <c r="U18" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="V18" s="5"/>
+      <c r="W18" s="17" t="s">
+        <v>84</v>
+      </c>
       <c r="X18" s="5"/>
-      <c r="Y18" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z18" s="5"/>
-      <c r="AA18" s="37">
+      <c r="Y18" s="37">
         <v>0.25</v>
       </c>
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="31"/>
       <c r="AB18" s="31"/>
       <c r="AC18" s="31"/>
       <c r="AD18" s="31"/>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31"/>
-    </row>
-    <row r="19" spans="1:32" ht="15" thickBot="1">
+    </row>
+    <row r="19" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="22" t="s">
         <v>132</v>
       </c>
@@ -3140,29 +3090,29 @@
       <c r="N19" s="34">
         <v>0</v>
       </c>
-      <c r="R19" s="34">
-        <v>1</v>
-      </c>
-      <c r="V19" s="32"/>
-      <c r="W19" s="72">
+      <c r="Q19" s="34">
+        <v>1</v>
+      </c>
+      <c r="T19" s="32"/>
+      <c r="U19" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="18" t="s">
+      <c r="V19" s="14"/>
+      <c r="W19" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="Z19" s="38"/>
-      <c r="AA19" s="39">
+      <c r="X19" s="38"/>
+      <c r="Y19" s="39">
         <v>0.05</v>
       </c>
+      <c r="Z19" s="31"/>
+      <c r="AA19" s="31"/>
       <c r="AB19" s="31"/>
       <c r="AC19" s="31"/>
       <c r="AD19" s="31"/>
-      <c r="AE19" s="31"/>
-      <c r="AF19" s="31"/>
-    </row>
-    <row r="20" spans="1:32">
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B20" s="22" t="s">
         <v>133</v>
       </c>
@@ -3173,19 +3123,19 @@
       <c r="N20" s="34">
         <v>0.5</v>
       </c>
-      <c r="V20" s="32"/>
-      <c r="W20" s="72">
+      <c r="T20" s="32"/>
+      <c r="U20" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="Z20" s="31"/>
+      <c r="AA20" s="31"/>
       <c r="AB20" s="31"/>
       <c r="AC20" s="31"/>
       <c r="AD20" s="31"/>
-      <c r="AE20" s="31"/>
-      <c r="AF20" s="31"/>
-    </row>
-    <row r="21" spans="1:32" ht="15" thickBot="1">
+    </row>
+    <row r="21" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="22" t="s">
         <v>134</v>
       </c>
@@ -3196,22 +3146,22 @@
       <c r="N21" s="34">
         <v>0</v>
       </c>
-      <c r="V21" s="32"/>
-      <c r="W21" s="72">
+      <c r="T21" s="32"/>
+      <c r="U21" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X21" s="14"/>
-      <c r="Y21" s="14"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="14"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="31"/>
+      <c r="AA21" s="31"/>
       <c r="AB21" s="31"/>
       <c r="AC21" s="31"/>
       <c r="AD21" s="31"/>
-      <c r="AE21" s="31"/>
-      <c r="AF21" s="31"/>
-    </row>
-    <row r="22" spans="1:32">
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B22" s="22" t="s">
         <v>135</v>
       </c>
@@ -3222,30 +3172,30 @@
       <c r="N22" s="34">
         <v>0.1</v>
       </c>
-      <c r="V22" s="32"/>
-      <c r="W22" s="72">
+      <c r="T22" s="32"/>
+      <c r="U22" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X22" s="14"/>
-      <c r="Y22" s="44" t="s">
+      <c r="V22" s="14"/>
+      <c r="W22" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="Z22" s="4" t="s">
+      <c r="X22" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AA22" s="4" t="s">
+      <c r="Y22" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AB22" s="7" t="s">
+      <c r="Z22" s="7" t="s">
         <v>106</v>
       </c>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="31"/>
       <c r="AC22" s="31"/>
       <c r="AD22" s="31"/>
-      <c r="AE22" s="31"/>
-      <c r="AF22" s="31"/>
-    </row>
-    <row r="23" spans="1:32">
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B23" s="22" t="s">
         <v>136</v>
       </c>
@@ -3256,33 +3206,33 @@
       <c r="N23" s="34">
         <v>0</v>
       </c>
-      <c r="V23" s="32"/>
-      <c r="W23" s="72">
+      <c r="T23" s="32"/>
+      <c r="U23" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X23" s="14"/>
-      <c r="Y23" s="74">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="6">
-        <f t="shared" ref="Z23:Z31" si="1">SUMIF(W$2:W$82,"&gt;=" &amp; Y23,C$2:C$82)</f>
+      <c r="V23" s="14"/>
+      <c r="W23" s="74">
+        <v>0</v>
+      </c>
+      <c r="X23" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W23,C$2:C$82)</f>
         <v>330</v>
       </c>
-      <c r="AA23" s="6">
-        <f t="shared" ref="AA23:AA31" si="2">SUMIF(W$2:W$82,"&gt;=" &amp; Y23,D$2:D$82)</f>
+      <c r="Y23" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W23,D$2:D$82)</f>
         <v>11</v>
       </c>
-      <c r="AB23" s="8">
-        <f t="shared" ref="AB23:AB31" si="3">($AA$17 + $AA$15*Z23+$AA$16*AA23)*(1+AA$18+AA$19)</f>
+      <c r="Z23" s="8">
+        <f t="shared" ref="Z23:Z31" si="1">($Y$17 + $Y$15*X23+$Y$16*Y23)*(1+Y$18+Y$19)</f>
         <v>29.64</v>
       </c>
+      <c r="AA23" s="31"/>
+      <c r="AB23" s="31"/>
       <c r="AC23" s="31"/>
       <c r="AD23" s="31"/>
-      <c r="AE23" s="31"/>
-      <c r="AF23" s="31"/>
-    </row>
-    <row r="24" spans="1:32" s="6" customFormat="1">
+    </row>
+    <row r="24" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="22" t="s">
         <v>137</v>
@@ -3332,39 +3282,33 @@
       <c r="S24" s="34">
         <v>1</v>
       </c>
-      <c r="T24" s="34">
-        <v>1</v>
-      </c>
-      <c r="U24" s="34">
-        <v>1</v>
-      </c>
-      <c r="V24" s="32"/>
-      <c r="W24" s="72">
+      <c r="T24" s="32"/>
+      <c r="U24" s="72">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="X24" s="14"/>
-      <c r="Y24" s="74">
+      <c r="V24" s="14"/>
+      <c r="W24" s="74">
         <v>0.5</v>
       </c>
-      <c r="Z24" s="6">
+      <c r="X24" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W24,C$2:C$82)</f>
+        <v>231</v>
+      </c>
+      <c r="Y24" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W24,D$2:D$82)</f>
+        <v>5</v>
+      </c>
+      <c r="Z24" s="8">
         <f t="shared" si="1"/>
-        <v>234</v>
-      </c>
-      <c r="AA24" s="6">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="AB24" s="8">
-        <f t="shared" si="3"/>
-        <v>21.060000000000006</v>
-      </c>
+        <v>20.865000000000002</v>
+      </c>
+      <c r="AA24" s="31"/>
+      <c r="AB24" s="31"/>
       <c r="AC24" s="31"/>
       <c r="AD24" s="31"/>
-      <c r="AE24" s="31"/>
-      <c r="AF24" s="31"/>
-    </row>
-    <row r="25" spans="1:32">
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B25" s="22" t="s">
         <v>138</v>
       </c>
@@ -3387,43 +3331,40 @@
         <v>1</v>
       </c>
       <c r="O25" s="34">
-        <v>0.75</v>
-      </c>
-      <c r="P25" s="34">
-        <v>1</v>
-      </c>
-      <c r="T25" s="34">
+        <v>1</v>
+      </c>
+      <c r="R25" s="34">
         <v>0.5</v>
       </c>
-      <c r="V25" s="32">
-        <v>1</v>
-      </c>
-      <c r="W25" s="72">
+      <c r="T25" s="32">
+        <v>1</v>
+      </c>
+      <c r="U25" s="72">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="74">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="6">
+      <c r="V25" s="14"/>
+      <c r="W25" s="74">
+        <v>1</v>
+      </c>
+      <c r="X25" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W25,C$2:C$82)</f>
+        <v>177</v>
+      </c>
+      <c r="Y25" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W25,D$2:D$82)</f>
+        <v>2</v>
+      </c>
+      <c r="Z25" s="8">
         <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="AA25" s="6">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="AB25" s="8">
-        <f t="shared" si="3"/>
-        <v>16.38</v>
-      </c>
+        <v>16.184999999999999</v>
+      </c>
+      <c r="AA25" s="31"/>
+      <c r="AB25" s="31"/>
       <c r="AC25" s="31"/>
       <c r="AD25" s="31"/>
-      <c r="AE25" s="31"/>
-      <c r="AF25" s="31"/>
-    </row>
-    <row r="26" spans="1:32">
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B26" s="22" t="s">
         <v>139</v>
       </c>
@@ -3458,39 +3399,36 @@
       <c r="P26" s="34">
         <v>1</v>
       </c>
-      <c r="Q26" s="34">
-        <v>1</v>
-      </c>
-      <c r="T26" s="34">
-        <v>1</v>
-      </c>
-      <c r="V26" s="32"/>
-      <c r="W26" s="72">
+      <c r="R26" s="34">
+        <v>1</v>
+      </c>
+      <c r="T26" s="32"/>
+      <c r="U26" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X26" s="14"/>
-      <c r="Y26" s="75">
+      <c r="V26" s="14"/>
+      <c r="W26" s="75">
         <v>1.5</v>
       </c>
-      <c r="Z26" s="29">
+      <c r="X26" s="29">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W26,C$2:C$82)</f>
+        <v>41</v>
+      </c>
+      <c r="Y26" s="29">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W26,D$2:D$82)</f>
+        <v>1</v>
+      </c>
+      <c r="Z26" s="8">
         <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="AA26" s="29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AB26" s="8">
-        <f t="shared" si="3"/>
         <v>6.955000000000001</v>
       </c>
+      <c r="AA26" s="31"/>
+      <c r="AB26" s="31"/>
       <c r="AC26" s="31"/>
       <c r="AD26" s="31"/>
-      <c r="AE26" s="31"/>
-      <c r="AF26" s="31"/>
-    </row>
-    <row r="27" spans="1:32">
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>117</v>
       </c>
@@ -3540,33 +3478,29 @@
         <v>1</v>
       </c>
       <c r="S27" s="33"/>
-      <c r="T27" s="33">
-        <v>1</v>
-      </c>
-      <c r="U27" s="33"/>
-      <c r="V27" s="33"/>
-      <c r="W27" s="72">
+      <c r="T27" s="33"/>
+      <c r="U27" s="81">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="74">
+      <c r="V27" s="14"/>
+      <c r="W27" s="74">
         <v>2</v>
       </c>
-      <c r="Z27" s="6">
+      <c r="X27" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W27,C$2:C$82)</f>
+        <v>37</v>
+      </c>
+      <c r="Y27" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W27,D$2:D$82)</f>
+        <v>1</v>
+      </c>
+      <c r="Z27" s="8">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="AA27" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AB27" s="8">
-        <f t="shared" si="3"/>
         <v>6.6949999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:32">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B28" s="22" t="s">
         <v>141</v>
       </c>
@@ -3604,32 +3538,29 @@
       <c r="R28" s="34">
         <v>1</v>
       </c>
-      <c r="T28" s="34">
-        <v>1</v>
-      </c>
-      <c r="V28" s="32"/>
-      <c r="W28" s="72">
+      <c r="T28" s="32"/>
+      <c r="U28" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X28" s="14"/>
-      <c r="Y28" s="74">
+      <c r="V28" s="14"/>
+      <c r="W28" s="74">
         <v>2.5</v>
       </c>
-      <c r="Z28" s="6">
+      <c r="X28" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W28,C$2:C$82)</f>
+        <v>11</v>
+      </c>
+      <c r="Y28" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W28,D$2:D$82)</f>
+        <v>1</v>
+      </c>
+      <c r="Z28" s="8">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="AA28" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AB28" s="8">
-        <f t="shared" si="3"/>
         <v>5.0049999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:32">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B29" s="22" t="s">
         <v>142</v>
       </c>
@@ -3646,35 +3577,32 @@
       <c r="O29" s="34">
         <v>0.75</v>
       </c>
-      <c r="P29" s="34">
-        <v>0.75</v>
-      </c>
-      <c r="T29" s="34">
+      <c r="R29" s="34">
         <v>0.5</v>
       </c>
-      <c r="V29" s="32"/>
-      <c r="W29" s="72">
+      <c r="T29" s="32"/>
+      <c r="U29" s="72">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="74">
+      <c r="V29" s="14"/>
+      <c r="W29" s="74">
         <v>3</v>
       </c>
-      <c r="Z29" s="6">
+      <c r="X29" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W29,C$2:C$82)</f>
+        <v>11</v>
+      </c>
+      <c r="Y29" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W29,D$2:D$82)</f>
+        <v>1</v>
+      </c>
+      <c r="Z29" s="8">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="AA29" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AB29" s="8">
-        <f t="shared" si="3"/>
         <v>5.0049999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:32">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B30" s="22" t="s">
         <v>143</v>
       </c>
@@ -3701,43 +3629,40 @@
         <v>0.9</v>
       </c>
       <c r="O30" s="34">
+        <v>1</v>
+      </c>
+      <c r="P30" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="34">
+        <v>1</v>
+      </c>
+      <c r="R30" s="34">
         <v>0.75</v>
       </c>
-      <c r="P30" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="34">
-        <v>1</v>
-      </c>
-      <c r="R30" s="34">
-        <v>1</v>
-      </c>
-      <c r="T30" s="34">
-        <v>0.75</v>
-      </c>
-      <c r="V30" s="32"/>
-      <c r="W30" s="72">
+      <c r="T30" s="32"/>
+      <c r="U30" s="72">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="X30" s="14"/>
-      <c r="Y30" s="74">
+      <c r="V30" s="14"/>
+      <c r="W30" s="74">
         <v>3.5</v>
       </c>
-      <c r="Z30" s="6">
+      <c r="X30" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W30,C$2:C$82)</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="6">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W30,D$2:D$82)</f>
+        <v>0</v>
+      </c>
+      <c r="Z30" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AA30" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB30" s="8">
-        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:32" ht="15" thickBot="1">
+    <row r="31" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="22" t="s">
         <v>191</v>
       </c>
@@ -3753,35 +3678,32 @@
       <c r="O31" s="34">
         <v>1</v>
       </c>
-      <c r="P31" s="34">
-        <v>1</v>
-      </c>
-      <c r="T31" s="34">
+      <c r="R31" s="34">
         <v>0.5</v>
       </c>
-      <c r="V31" s="32"/>
-      <c r="W31" s="72">
+      <c r="T31" s="32"/>
+      <c r="U31" s="72">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="X31" s="14"/>
-      <c r="Y31" s="76">
+      <c r="V31" s="14"/>
+      <c r="W31" s="76">
         <v>4</v>
       </c>
-      <c r="Z31" s="45">
+      <c r="X31" s="45">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W31,C$2:C$82)</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="45">
+        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W31,D$2:D$82)</f>
+        <v>0</v>
+      </c>
+      <c r="Z31" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AA31" s="45">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB31" s="9">
-        <f t="shared" si="3"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:32" s="6" customFormat="1">
+    <row r="32" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="22" t="s">
         <v>144</v>
@@ -3822,26 +3744,22 @@
       <c r="P32" s="34">
         <v>1</v>
       </c>
-      <c r="Q32" s="34">
-        <v>1</v>
-      </c>
-      <c r="R32" s="34"/>
+      <c r="Q32" s="34"/>
+      <c r="R32" s="34">
+        <v>1</v>
+      </c>
       <c r="S32" s="34"/>
-      <c r="T32" s="34">
-        <v>1</v>
-      </c>
-      <c r="U32" s="34"/>
-      <c r="V32" s="32"/>
-      <c r="W32" s="72">
+      <c r="T32" s="32"/>
+      <c r="U32" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X32" s="14"/>
-      <c r="Y32" s="3"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-    </row>
-    <row r="33" spans="1:32">
+      <c r="V32" s="14"/>
+      <c r="W32" s="3"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B33" s="22" t="s">
         <v>145</v>
       </c>
@@ -3856,25 +3774,22 @@
         <v>0</v>
       </c>
       <c r="O33" s="34">
-        <v>0.75</v>
-      </c>
-      <c r="P33" s="34">
         <v>0.5</v>
       </c>
+      <c r="Q33" s="34">
+        <v>1</v>
+      </c>
       <c r="R33" s="34">
-        <v>1</v>
-      </c>
-      <c r="T33" s="34">
         <v>0.5</v>
       </c>
-      <c r="V33" s="32"/>
-      <c r="W33" s="72">
+      <c r="T33" s="32"/>
+      <c r="U33" s="72">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="X33" s="14"/>
-    </row>
-    <row r="34" spans="1:32">
+      <c r="V33" s="14"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B34" s="22" t="s">
         <v>146</v>
       </c>
@@ -3912,20 +3827,17 @@
       <c r="P34" s="34">
         <v>1</v>
       </c>
-      <c r="Q34" s="34">
-        <v>1</v>
-      </c>
-      <c r="T34" s="34">
-        <v>1</v>
-      </c>
-      <c r="V34" s="32"/>
-      <c r="W34" s="72">
+      <c r="R34" s="34">
+        <v>1</v>
+      </c>
+      <c r="T34" s="32"/>
+      <c r="U34" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X34" s="14"/>
-    </row>
-    <row r="35" spans="1:32">
+      <c r="V34" s="14"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B35" s="22" t="s">
         <v>147</v>
       </c>
@@ -3947,17 +3859,17 @@
       <c r="N35" s="34">
         <v>1</v>
       </c>
-      <c r="V35" s="32">
-        <v>1</v>
-      </c>
-      <c r="W35" s="72">
+      <c r="T35" s="32">
+        <v>1</v>
+      </c>
+      <c r="U35" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X35" s="14"/>
-      <c r="Y35" s="77"/>
-    </row>
-    <row r="36" spans="1:32" s="31" customFormat="1">
+      <c r="V35" s="14"/>
+      <c r="W35" s="77"/>
+    </row>
+    <row r="36" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="22" t="s">
         <v>194</v>
@@ -3982,22 +3894,20 @@
       </c>
       <c r="O36" s="34"/>
       <c r="P36" s="34"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34">
-        <v>1</v>
-      </c>
+      <c r="Q36" s="34">
+        <v>1</v>
+      </c>
+      <c r="R36" s="34"/>
       <c r="S36" s="34"/>
-      <c r="T36" s="34"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="32"/>
-      <c r="W36" s="72">
+      <c r="T36" s="32"/>
+      <c r="U36" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X36" s="14"/>
-      <c r="Y36" s="77"/>
-    </row>
-    <row r="37" spans="1:32">
+      <c r="V36" s="14"/>
+      <c r="W36" s="77"/>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B37" s="22" t="s">
         <v>148</v>
       </c>
@@ -4027,26 +3937,23 @@
         <v>0</v>
       </c>
       <c r="O37" s="34">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="P37" s="34">
+        <v>1</v>
+      </c>
+      <c r="R37" s="34">
         <v>0.5</v>
       </c>
-      <c r="Q37" s="34">
-        <v>1</v>
-      </c>
-      <c r="T37" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="V37" s="32"/>
-      <c r="W37" s="72">
+      <c r="T37" s="32"/>
+      <c r="U37" s="72">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="X37" s="14"/>
-      <c r="Y37" s="77"/>
-    </row>
-    <row r="38" spans="1:32" s="31" customFormat="1">
+      <c r="V37" s="14"/>
+      <c r="W37" s="77"/>
+    </row>
+    <row r="38" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="22" t="s">
         <v>149</v>
@@ -4085,24 +3992,20 @@
       <c r="P38" s="34">
         <v>1</v>
       </c>
-      <c r="Q38" s="34">
-        <v>1</v>
-      </c>
-      <c r="R38" s="34"/>
+      <c r="Q38" s="34"/>
+      <c r="R38" s="34">
+        <v>1</v>
+      </c>
       <c r="S38" s="34"/>
-      <c r="T38" s="34">
-        <v>1</v>
-      </c>
-      <c r="U38" s="34"/>
-      <c r="V38" s="32"/>
-      <c r="W38" s="72">
+      <c r="T38" s="32"/>
+      <c r="U38" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X38" s="14"/>
-      <c r="Y38" s="77"/>
-    </row>
-    <row r="39" spans="1:32">
+      <c r="V38" s="14"/>
+      <c r="W38" s="77"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B39" s="22" t="s">
         <v>150</v>
       </c>
@@ -4128,19 +4031,16 @@
       <c r="N39" s="34">
         <v>0</v>
       </c>
-      <c r="O39" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="V39" s="32"/>
-      <c r="W39" s="72">
+      <c r="T39" s="32"/>
+      <c r="U39" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X39" s="14"/>
-      <c r="Y39" s="77"/>
-      <c r="AB39" s="6"/>
-    </row>
-    <row r="40" spans="1:32">
+      <c r="V39" s="14"/>
+      <c r="W39" s="77"/>
+      <c r="Z39" s="6"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B40" s="22" t="s">
         <v>180</v>
       </c>
@@ -4156,14 +4056,14 @@
       <c r="N40" s="34">
         <v>0</v>
       </c>
-      <c r="V40" s="32"/>
-      <c r="W40" s="72">
+      <c r="T40" s="32"/>
+      <c r="U40" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X40" s="14"/>
-    </row>
-    <row r="41" spans="1:32">
+      <c r="V40" s="14"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>116</v>
       </c>
@@ -4208,25 +4108,21 @@
       <c r="P41" s="33">
         <v>1</v>
       </c>
-      <c r="Q41" s="33">
-        <v>1</v>
-      </c>
-      <c r="R41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33">
+        <v>0.75</v>
+      </c>
       <c r="S41" s="33"/>
-      <c r="T41" s="33">
-        <v>0.75</v>
-      </c>
-      <c r="U41" s="33"/>
-      <c r="V41" s="33"/>
-      <c r="W41" s="72">
+      <c r="T41" s="33"/>
+      <c r="U41" s="81">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="X41" s="14"/>
-      <c r="Y41" s="14"/>
-      <c r="Z41" s="6"/>
-    </row>
-    <row r="42" spans="1:32" s="6" customFormat="1">
+      <c r="V41" s="14"/>
+      <c r="W41" s="14"/>
+      <c r="X41" s="6"/>
+    </row>
+    <row r="42" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="28"/>
       <c r="B42" s="29" t="s">
         <v>152</v>
@@ -4276,25 +4172,21 @@
         <v>1</v>
       </c>
       <c r="S42" s="34"/>
-      <c r="T42" s="34">
-        <v>1</v>
-      </c>
-      <c r="U42" s="34"/>
-      <c r="V42" s="34"/>
-      <c r="W42" s="72">
+      <c r="T42" s="34"/>
+      <c r="U42" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X42" s="14"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="3"/>
+      <c r="X42"/>
+      <c r="Y42"/>
       <c r="AA42"/>
+      <c r="AB42"/>
       <c r="AC42"/>
       <c r="AD42"/>
-      <c r="AE42"/>
-      <c r="AF42"/>
-    </row>
-    <row r="43" spans="1:32">
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A43" s="28"/>
       <c r="B43" s="29" t="s">
         <v>153</v>
@@ -4333,30 +4225,24 @@
       <c r="P43" s="34">
         <v>1</v>
       </c>
-      <c r="Q43" s="34">
+      <c r="R43" s="34">
         <v>1</v>
       </c>
       <c r="S43" s="34">
         <v>1</v>
       </c>
-      <c r="T43" s="34">
-        <v>1</v>
-      </c>
-      <c r="U43" s="34">
-        <v>1</v>
-      </c>
-      <c r="V43" s="34"/>
-      <c r="W43" s="72">
+      <c r="T43" s="34"/>
+      <c r="U43" s="72">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="X43" s="14"/>
+      <c r="V43" s="14"/>
+      <c r="AA43" s="6"/>
+      <c r="AB43" s="6"/>
       <c r="AC43" s="6"/>
       <c r="AD43" s="6"/>
-      <c r="AE43" s="6"/>
-      <c r="AF43" s="6"/>
-    </row>
-    <row r="44" spans="1:32">
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A44" s="28"/>
       <c r="B44" s="29" t="s">
         <v>154</v>
@@ -4374,18 +4260,18 @@
       <c r="N44" s="34">
         <v>0</v>
       </c>
-      <c r="Q44" s="34">
+      <c r="P44" s="34">
         <v>0.5</v>
       </c>
-      <c r="V44" s="34"/>
-      <c r="W44" s="72">
+      <c r="T44" s="34"/>
+      <c r="U44" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X44" s="14"/>
-      <c r="AB44" s="6"/>
-    </row>
-    <row r="45" spans="1:32">
+      <c r="V44" s="14"/>
+      <c r="Z44" s="6"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A45" s="28"/>
       <c r="B45" s="29" t="s">
         <v>155</v>
@@ -4418,19 +4304,16 @@
       <c r="N45" s="34">
         <v>1</v>
       </c>
-      <c r="O45" s="34">
-        <v>1</v>
-      </c>
-      <c r="V45" s="34"/>
-      <c r="W45" s="72">
+      <c r="T45" s="34"/>
+      <c r="U45" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X45" s="14"/>
-      <c r="Y45" s="14"/>
-      <c r="Z45" s="6"/>
-    </row>
-    <row r="46" spans="1:32">
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="6"/>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A46" s="28"/>
       <c r="B46" s="29" t="s">
         <v>156</v>
@@ -4472,18 +4355,15 @@
       <c r="R46" s="34">
         <v>1</v>
       </c>
-      <c r="T46" s="34">
-        <v>1</v>
-      </c>
-      <c r="V46" s="34"/>
-      <c r="W46" s="72">
+      <c r="T46" s="34"/>
+      <c r="U46" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X46" s="14"/>
-      <c r="AA46" s="6"/>
-    </row>
-    <row r="47" spans="1:32" s="6" customFormat="1">
+      <c r="V46" s="14"/>
+      <c r="Y46" s="6"/>
+    </row>
+    <row r="47" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="28"/>
       <c r="B47" s="29" t="s">
         <v>157</v>
@@ -4522,31 +4402,27 @@
       <c r="P47" s="34">
         <v>1</v>
       </c>
-      <c r="Q47" s="34">
-        <v>1</v>
-      </c>
-      <c r="R47" s="34"/>
+      <c r="Q47" s="34"/>
+      <c r="R47" s="34">
+        <v>1</v>
+      </c>
       <c r="S47" s="34"/>
-      <c r="T47" s="34">
-        <v>1</v>
-      </c>
-      <c r="U47" s="34"/>
-      <c r="V47" s="34"/>
-      <c r="W47" s="72">
+      <c r="T47" s="34"/>
+      <c r="U47" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X47" s="14"/>
-      <c r="Y47" s="3"/>
+      <c r="V47" s="14"/>
+      <c r="W47" s="3"/>
+      <c r="X47"/>
+      <c r="Y47"/>
       <c r="Z47"/>
       <c r="AA47"/>
       <c r="AB47"/>
       <c r="AC47"/>
       <c r="AD47"/>
-      <c r="AE47"/>
-      <c r="AF47"/>
-    </row>
-    <row r="48" spans="1:32">
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A48" s="28"/>
       <c r="B48" s="29" t="s">
         <v>158</v>
@@ -4585,20 +4461,17 @@
       <c r="P48" s="34">
         <v>1</v>
       </c>
-      <c r="Q48" s="34">
-        <v>1</v>
-      </c>
-      <c r="T48" s="34">
-        <v>1</v>
-      </c>
-      <c r="V48" s="34"/>
-      <c r="W48" s="72">
+      <c r="R48" s="34">
+        <v>1</v>
+      </c>
+      <c r="T48" s="34"/>
+      <c r="U48" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X48" s="14"/>
-    </row>
-    <row r="49" spans="1:32">
+      <c r="V48" s="14"/>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A49" s="28"/>
       <c r="B49" s="29" t="s">
         <v>159</v>
@@ -4637,20 +4510,17 @@
       <c r="P49" s="34">
         <v>1</v>
       </c>
-      <c r="Q49" s="34">
-        <v>1</v>
-      </c>
-      <c r="T49" s="34">
-        <v>1</v>
-      </c>
-      <c r="V49" s="34"/>
-      <c r="W49" s="72">
+      <c r="R49" s="34">
+        <v>1</v>
+      </c>
+      <c r="T49" s="34"/>
+      <c r="U49" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X49" s="14"/>
-    </row>
-    <row r="50" spans="1:32" s="6" customFormat="1">
+      <c r="V49" s="14"/>
+    </row>
+    <row r="50" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="22" t="s">
         <v>160</v>
@@ -4689,37 +4559,31 @@
         <v>1</v>
       </c>
       <c r="P50" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q50" s="34">
         <v>0.5</v>
       </c>
-      <c r="R50" s="34"/>
+      <c r="Q50" s="34"/>
+      <c r="R50" s="34">
+        <v>1</v>
+      </c>
       <c r="S50" s="34">
         <v>1</v>
       </c>
-      <c r="T50" s="34">
-        <v>1</v>
-      </c>
-      <c r="U50" s="34">
-        <v>1</v>
-      </c>
-      <c r="V50" s="32">
-        <v>1</v>
-      </c>
-      <c r="W50" s="72">
+      <c r="T50" s="32">
+        <v>1</v>
+      </c>
+      <c r="U50" s="72">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="X50" s="14"/>
-      <c r="Y50" s="14"/>
+      <c r="V50" s="14"/>
+      <c r="W50" s="14"/>
+      <c r="Z50"/>
+      <c r="AA50"/>
       <c r="AB50"/>
       <c r="AC50"/>
       <c r="AD50"/>
-      <c r="AE50"/>
-      <c r="AF50"/>
-    </row>
-    <row r="51" spans="1:32">
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>115</v>
       </c>
@@ -4755,30 +4619,26 @@
         <v>0</v>
       </c>
       <c r="O51" s="33">
-        <v>0.75</v>
-      </c>
-      <c r="P51" s="33">
         <v>0.5</v>
       </c>
+      <c r="P51" s="33"/>
       <c r="Q51" s="33"/>
-      <c r="R51" s="33"/>
+      <c r="R51" s="33">
+        <v>0.5</v>
+      </c>
       <c r="S51" s="33"/>
-      <c r="T51" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="U51" s="33"/>
-      <c r="V51" s="33"/>
-      <c r="W51" s="72">
+      <c r="T51" s="33"/>
+      <c r="U51" s="81">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="X51" s="14"/>
-      <c r="AC51" s="31"/>
+      <c r="V51" s="14"/>
+      <c r="AA51" s="31"/>
+      <c r="AB51" s="6"/>
+      <c r="AC51" s="6"/>
       <c r="AD51" s="6"/>
-      <c r="AE51" s="6"/>
-      <c r="AF51" s="6"/>
-    </row>
-    <row r="52" spans="1:32" s="6" customFormat="1">
+    </row>
+    <row r="52" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="22" t="s">
         <v>162</v>
@@ -4826,26 +4686,22 @@
         <v>1</v>
       </c>
       <c r="S52" s="34"/>
-      <c r="T52" s="34">
-        <v>1</v>
-      </c>
-      <c r="U52" s="34"/>
-      <c r="V52" s="32"/>
-      <c r="W52" s="72">
+      <c r="T52" s="32"/>
+      <c r="U52" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X52" s="14"/>
-      <c r="Y52" s="3"/>
+      <c r="V52" s="14"/>
+      <c r="W52" s="3"/>
+      <c r="X52"/>
+      <c r="Y52"/>
       <c r="Z52"/>
-      <c r="AA52"/>
+      <c r="AA52" s="31"/>
       <c r="AB52"/>
-      <c r="AC52" s="31"/>
+      <c r="AC52"/>
       <c r="AD52"/>
-      <c r="AE52"/>
-      <c r="AF52"/>
-    </row>
-    <row r="53" spans="1:32" s="6" customFormat="1">
+    </row>
+    <row r="53" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="22" t="s">
         <v>193</v>
@@ -4868,31 +4724,29 @@
       <c r="N53" s="34">
         <v>1</v>
       </c>
-      <c r="O53" s="34"/>
-      <c r="P53" s="34">
+      <c r="O53" s="34">
         <v>0.5</v>
       </c>
+      <c r="P53" s="34"/>
       <c r="Q53" s="34"/>
       <c r="R53" s="34"/>
       <c r="S53" s="34"/>
-      <c r="T53" s="34"/>
-      <c r="U53" s="34"/>
-      <c r="V53" s="32"/>
-      <c r="W53" s="72">
+      <c r="T53" s="32"/>
+      <c r="U53" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X53" s="14"/>
-      <c r="Y53" s="3"/>
+      <c r="V53" s="14"/>
+      <c r="W53" s="3"/>
+      <c r="X53" s="31"/>
+      <c r="Y53" s="31"/>
       <c r="Z53" s="31"/>
       <c r="AA53" s="31"/>
       <c r="AB53" s="31"/>
       <c r="AC53" s="31"/>
       <c r="AD53" s="31"/>
-      <c r="AE53" s="31"/>
-      <c r="AF53" s="31"/>
-    </row>
-    <row r="54" spans="1:32">
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B54" s="22" t="s">
         <v>189</v>
       </c>
@@ -4905,27 +4759,24 @@
       <c r="N54" s="34">
         <v>1</v>
       </c>
-      <c r="P54" s="34">
-        <v>1</v>
-      </c>
-      <c r="R54" s="34">
+      <c r="O54" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="34">
         <v>1</v>
       </c>
       <c r="S54" s="34">
         <v>1</v>
       </c>
-      <c r="U54" s="34">
-        <v>1</v>
-      </c>
-      <c r="V54" s="32"/>
-      <c r="W54" s="72">
+      <c r="T54" s="32"/>
+      <c r="U54" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X54" s="14"/>
-      <c r="AC54" s="31"/>
-    </row>
-    <row r="55" spans="1:32">
+      <c r="V54" s="14"/>
+      <c r="AA54" s="31"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B55" s="22" t="s">
         <v>163</v>
       </c>
@@ -4969,18 +4820,15 @@
       <c r="R55" s="34">
         <v>1</v>
       </c>
-      <c r="T55" s="34">
-        <v>1</v>
-      </c>
-      <c r="V55" s="32"/>
-      <c r="W55" s="72">
+      <c r="T55" s="32"/>
+      <c r="U55" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X55" s="14"/>
-      <c r="AC55" s="31"/>
-    </row>
-    <row r="56" spans="1:32" s="31" customFormat="1">
+      <c r="V55" s="14"/>
+      <c r="AA55" s="31"/>
+    </row>
+    <row r="56" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
       <c r="B56" s="22" t="s">
         <v>164</v>
@@ -5003,24 +4851,20 @@
       <c r="N56" s="34">
         <v>0.5</v>
       </c>
-      <c r="O56" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="O56" s="34"/>
       <c r="P56" s="34"/>
       <c r="Q56" s="34"/>
       <c r="R56" s="34"/>
       <c r="S56" s="34"/>
-      <c r="T56" s="34"/>
-      <c r="U56" s="34"/>
-      <c r="V56" s="32"/>
-      <c r="W56" s="72">
+      <c r="T56" s="32"/>
+      <c r="U56" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X56" s="14"/>
-      <c r="Y56" s="3"/>
-    </row>
-    <row r="57" spans="1:32" s="31" customFormat="1">
+      <c r="V56" s="14"/>
+      <c r="W56" s="3"/>
+    </row>
+    <row r="57" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="10"/>
       <c r="B57" s="22" t="s">
         <v>165</v>
@@ -5043,22 +4887,20 @@
       </c>
       <c r="O57" s="34"/>
       <c r="P57" s="34"/>
-      <c r="Q57" s="34"/>
-      <c r="R57" s="34">
-        <v>1</v>
-      </c>
+      <c r="Q57" s="34">
+        <v>1</v>
+      </c>
+      <c r="R57" s="34"/>
       <c r="S57" s="34"/>
-      <c r="T57" s="34"/>
-      <c r="U57" s="34"/>
-      <c r="V57" s="32"/>
-      <c r="W57" s="72">
+      <c r="T57" s="32"/>
+      <c r="U57" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X57" s="14"/>
-      <c r="Y57" s="3"/>
-    </row>
-    <row r="58" spans="1:32">
+      <c r="V57" s="14"/>
+      <c r="W57" s="3"/>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B58" s="22" t="s">
         <v>183</v>
       </c>
@@ -5075,30 +4917,27 @@
         <v>0.7</v>
       </c>
       <c r="O58" s="34">
+        <v>1</v>
+      </c>
+      <c r="P58" s="34">
         <v>0.5</v>
       </c>
-      <c r="P58" s="34">
-        <v>1</v>
-      </c>
       <c r="Q58" s="34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R58" s="34">
         <v>1</v>
       </c>
-      <c r="T58" s="34">
-        <v>1</v>
-      </c>
-      <c r="V58" s="32"/>
-      <c r="W58" s="72">
+      <c r="T58" s="32"/>
+      <c r="U58" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X58" s="14"/>
-      <c r="AA58" s="6"/>
-      <c r="AC58" s="31"/>
-    </row>
-    <row r="59" spans="1:32">
+      <c r="V58" s="14"/>
+      <c r="Y58" s="6"/>
+      <c r="AA58" s="31"/>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B59" s="22" t="s">
         <v>166</v>
       </c>
@@ -5121,21 +4960,18 @@
       <c r="O59" s="34">
         <v>1</v>
       </c>
-      <c r="P59" s="34">
-        <v>1</v>
-      </c>
-      <c r="T59" s="34">
-        <v>1</v>
-      </c>
-      <c r="V59" s="32"/>
-      <c r="W59" s="72">
+      <c r="R59" s="34">
+        <v>1</v>
+      </c>
+      <c r="T59" s="32"/>
+      <c r="U59" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X59" s="14"/>
-      <c r="AC59" s="31"/>
-    </row>
-    <row r="60" spans="1:32">
+      <c r="V59" s="14"/>
+      <c r="AA59" s="31"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B60" s="22" t="s">
         <v>167</v>
       </c>
@@ -5179,19 +5015,16 @@
       <c r="R60" s="34">
         <v>1</v>
       </c>
-      <c r="T60" s="34">
-        <v>1</v>
-      </c>
-      <c r="V60" s="32"/>
-      <c r="W60" s="72">
+      <c r="T60" s="32"/>
+      <c r="U60" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X60" s="14"/>
-      <c r="AB60" s="6"/>
-      <c r="AC60" s="31"/>
-    </row>
-    <row r="61" spans="1:32">
+      <c r="V60" s="14"/>
+      <c r="Z60" s="6"/>
+      <c r="AA60" s="31"/>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>114</v>
       </c>
@@ -5230,24 +5063,20 @@
       <c r="P61" s="33">
         <v>1</v>
       </c>
-      <c r="Q61" s="33">
-        <v>1</v>
-      </c>
-      <c r="R61" s="33"/>
+      <c r="Q61" s="33"/>
+      <c r="R61" s="33">
+        <v>1</v>
+      </c>
       <c r="S61" s="33"/>
-      <c r="T61" s="33">
-        <v>1</v>
-      </c>
-      <c r="U61" s="33"/>
-      <c r="V61" s="33"/>
-      <c r="W61" s="72">
+      <c r="T61" s="33"/>
+      <c r="U61" s="81">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X61" s="14"/>
-      <c r="AC61" s="31"/>
-    </row>
-    <row r="62" spans="1:32">
+      <c r="V61" s="14"/>
+      <c r="AA61" s="31"/>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B62" s="22" t="s">
         <v>169</v>
       </c>
@@ -5291,24 +5120,21 @@
       <c r="R62" s="34">
         <v>1</v>
       </c>
-      <c r="T62" s="34">
-        <v>1</v>
-      </c>
-      <c r="V62" s="32"/>
-      <c r="W62" s="72">
+      <c r="T62" s="32"/>
+      <c r="U62" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X62" s="14"/>
-      <c r="AC62" s="31"/>
+      <c r="V62" s="14"/>
+      <c r="AA62" s="31"/>
+      <c r="AB62" s="6"/>
+      <c r="AC62" s="6"/>
       <c r="AD62" s="6"/>
-      <c r="AE62" s="6"/>
-      <c r="AF62" s="6"/>
-    </row>
-    <row r="63" spans="1:32" s="31" customFormat="1">
+    </row>
+    <row r="63" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10"/>
       <c r="B63" s="22" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C63" s="13">
         <v>2</v>
@@ -5319,7 +5145,7 @@
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
       <c r="I63" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J63" s="34"/>
       <c r="K63" s="34"/>
@@ -5327,28 +5153,26 @@
       <c r="M63" s="34"/>
       <c r="N63" s="34"/>
       <c r="O63" s="34"/>
-      <c r="P63" s="34"/>
-      <c r="Q63" s="34">
-        <v>1</v>
-      </c>
-      <c r="R63" s="34"/>
+      <c r="P63" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="34"/>
+      <c r="R63" s="34">
+        <v>0.75</v>
+      </c>
       <c r="S63" s="34"/>
-      <c r="T63" s="34">
-        <v>0.75</v>
-      </c>
-      <c r="U63" s="34"/>
-      <c r="V63" s="32"/>
-      <c r="W63" s="72">
+      <c r="T63" s="32"/>
+      <c r="U63" s="72">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="X63" s="14"/>
-      <c r="Y63" s="3"/>
+      <c r="V63" s="14"/>
+      <c r="W63" s="3"/>
+      <c r="AB63" s="6"/>
+      <c r="AC63" s="6"/>
       <c r="AD63" s="6"/>
-      <c r="AE63" s="6"/>
-      <c r="AF63" s="6"/>
-    </row>
-    <row r="64" spans="1:32">
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B64" s="22" t="s">
         <v>170</v>
       </c>
@@ -5383,24 +5207,21 @@
       <c r="O64" s="34">
         <v>1</v>
       </c>
-      <c r="P64" s="34">
+      <c r="Q64" s="34">
         <v>1</v>
       </c>
       <c r="R64" s="34">
         <v>1</v>
       </c>
-      <c r="T64" s="34">
-        <v>1</v>
-      </c>
-      <c r="V64" s="32"/>
-      <c r="W64" s="72">
+      <c r="T64" s="32"/>
+      <c r="U64" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="X64" s="14"/>
-      <c r="AC64" s="31"/>
-    </row>
-    <row r="65" spans="1:32" s="31" customFormat="1">
+      <c r="V64" s="14"/>
+      <c r="AA64" s="31"/>
+    </row>
+    <row r="65" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10"/>
       <c r="B65" s="22" t="s">
         <v>195</v>
@@ -5423,26 +5244,24 @@
       <c r="N65" s="34">
         <v>1</v>
       </c>
-      <c r="O65" s="34"/>
-      <c r="P65" s="34">
-        <v>1</v>
-      </c>
+      <c r="O65" s="34">
+        <v>1</v>
+      </c>
+      <c r="P65" s="34"/>
       <c r="Q65" s="34"/>
-      <c r="R65" s="34"/>
+      <c r="R65" s="34">
+        <v>0.5</v>
+      </c>
       <c r="S65" s="34"/>
-      <c r="T65" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="U65" s="34"/>
-      <c r="V65" s="32"/>
-      <c r="W65" s="72">
+      <c r="T65" s="32"/>
+      <c r="U65" s="72">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="X65" s="14"/>
-      <c r="Y65" s="3"/>
-    </row>
-    <row r="66" spans="1:32">
+      <c r="V65" s="14"/>
+      <c r="W65" s="3"/>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B66" s="22" t="s">
         <v>171</v>
       </c>
@@ -5453,16 +5272,16 @@
       <c r="N66" s="34">
         <v>0</v>
       </c>
-      <c r="V66" s="32"/>
-      <c r="W66" s="72">
+      <c r="T66" s="32"/>
+      <c r="U66" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X66" s="14"/>
-      <c r="AB66" s="6"/>
-      <c r="AC66" s="31"/>
-    </row>
-    <row r="67" spans="1:32">
+      <c r="V66" s="14"/>
+      <c r="Z66" s="6"/>
+      <c r="AA66" s="31"/>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>113</v>
       </c>
@@ -5492,23 +5311,21 @@
         <v>1</v>
       </c>
       <c r="O67" s="33"/>
-      <c r="P67" s="33"/>
-      <c r="Q67" s="33">
-        <v>1</v>
-      </c>
+      <c r="P67" s="33">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="33"/>
       <c r="R67" s="33"/>
       <c r="S67" s="33"/>
       <c r="T67" s="33"/>
-      <c r="U67" s="33"/>
-      <c r="V67" s="33"/>
-      <c r="W67" s="72">
-        <f t="shared" ref="W67:W81" si="4">SUM(T67:V67)</f>
-        <v>0</v>
-      </c>
-      <c r="X67" s="14"/>
-      <c r="AC67" s="31"/>
-    </row>
-    <row r="68" spans="1:32" s="31" customFormat="1">
+      <c r="U67" s="81">
+        <f t="shared" ref="U67:U81" si="2">SUM(R67:T67)</f>
+        <v>0</v>
+      </c>
+      <c r="V67" s="14"/>
+      <c r="AA67" s="31"/>
+    </row>
+    <row r="68" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="28"/>
       <c r="B68" s="29" t="s">
         <v>196</v>
@@ -5531,28 +5348,22 @@
       <c r="N68" s="34">
         <v>1</v>
       </c>
-      <c r="O68" s="34">
-        <v>1</v>
-      </c>
-      <c r="P68" s="34"/>
-      <c r="Q68" s="34">
+      <c r="O68" s="34"/>
+      <c r="P68" s="34">
         <v>0.5</v>
       </c>
+      <c r="Q68" s="34"/>
       <c r="R68" s="34"/>
       <c r="S68" s="34"/>
       <c r="T68" s="34"/>
-      <c r="U68" s="34"/>
-      <c r="V68" s="34">
-        <v>1</v>
-      </c>
-      <c r="W68" s="72">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="X68" s="14"/>
-      <c r="Y68" s="3"/>
-    </row>
-    <row r="69" spans="1:32" s="31" customFormat="1">
+      <c r="U68" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V68" s="14"/>
+      <c r="W68" s="3"/>
+    </row>
+    <row r="69" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="28"/>
       <c r="B69" s="29" t="s">
         <v>197</v>
@@ -5581,16 +5392,14 @@
       <c r="R69" s="34"/>
       <c r="S69" s="34"/>
       <c r="T69" s="34"/>
-      <c r="U69" s="34"/>
-      <c r="V69" s="34"/>
-      <c r="W69" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X69" s="14"/>
-      <c r="Y69" s="3"/>
-    </row>
-    <row r="70" spans="1:32" s="31" customFormat="1">
+      <c r="U69" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V69" s="14"/>
+      <c r="W69" s="3"/>
+    </row>
+    <row r="70" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="28"/>
       <c r="B70" s="29" t="s">
         <v>198</v>
@@ -5619,16 +5428,14 @@
       <c r="R70" s="34"/>
       <c r="S70" s="34"/>
       <c r="T70" s="34"/>
-      <c r="U70" s="34"/>
-      <c r="V70" s="34"/>
-      <c r="W70" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X70" s="14"/>
-      <c r="Y70" s="3"/>
-    </row>
-    <row r="71" spans="1:32" s="31" customFormat="1">
+      <c r="U70" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V70" s="14"/>
+      <c r="W70" s="3"/>
+    </row>
+    <row r="71" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="28"/>
       <c r="B71" s="29" t="s">
         <v>199</v>
@@ -5651,24 +5458,20 @@
       <c r="N71" s="34">
         <v>0.9</v>
       </c>
-      <c r="O71" s="34">
-        <v>1</v>
-      </c>
+      <c r="O71" s="34"/>
       <c r="P71" s="34"/>
       <c r="Q71" s="34"/>
       <c r="R71" s="34"/>
       <c r="S71" s="34"/>
       <c r="T71" s="34"/>
-      <c r="U71" s="34"/>
-      <c r="V71" s="34"/>
-      <c r="W71" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X71" s="14"/>
-      <c r="Y71" s="3"/>
-    </row>
-    <row r="72" spans="1:32">
+      <c r="U71" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V71" s="14"/>
+      <c r="W71" s="3"/>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B72" s="22" t="s">
         <v>173</v>
       </c>
@@ -5688,17 +5491,17 @@
       <c r="N72" s="34">
         <v>0</v>
       </c>
-      <c r="Q72" s="34">
-        <v>1</v>
-      </c>
-      <c r="V72" s="32"/>
-      <c r="W72" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X72" s="14"/>
-    </row>
-    <row r="73" spans="1:32">
+      <c r="P72" s="34">
+        <v>1</v>
+      </c>
+      <c r="T72" s="32"/>
+      <c r="U72" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V72" s="14"/>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>74</v>
       </c>
@@ -5735,21 +5538,17 @@
       <c r="P73" s="33">
         <v>1</v>
       </c>
-      <c r="Q73" s="33">
-        <v>1</v>
-      </c>
+      <c r="Q73" s="33"/>
       <c r="R73" s="33"/>
       <c r="S73" s="33"/>
       <c r="T73" s="33"/>
-      <c r="U73" s="33"/>
-      <c r="V73" s="33"/>
-      <c r="W73" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X73" s="14"/>
-    </row>
-    <row r="74" spans="1:32" s="6" customFormat="1">
+      <c r="U73" s="81">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V73" s="14"/>
+    </row>
+    <row r="74" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="28"/>
       <c r="B74" s="29" t="s">
         <v>82</v>
@@ -5784,29 +5583,25 @@
       <c r="P74" s="34">
         <v>1</v>
       </c>
-      <c r="Q74" s="34">
-        <v>1</v>
-      </c>
+      <c r="Q74" s="34"/>
       <c r="R74" s="34"/>
       <c r="S74" s="34"/>
       <c r="T74" s="34"/>
-      <c r="U74" s="34"/>
-      <c r="V74" s="34"/>
-      <c r="W74" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X74" s="14"/>
-      <c r="Y74" s="3"/>
+      <c r="U74" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V74" s="14"/>
+      <c r="W74" s="3"/>
+      <c r="X74"/>
+      <c r="Y74"/>
       <c r="Z74"/>
       <c r="AA74"/>
       <c r="AB74"/>
       <c r="AC74"/>
       <c r="AD74"/>
-      <c r="AE74"/>
-      <c r="AF74"/>
-    </row>
-    <row r="75" spans="1:32">
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B75" s="22" t="s">
         <v>93</v>
       </c>
@@ -5819,16 +5614,16 @@
       <c r="I75" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="V75" s="32"/>
-      <c r="W75" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X75" s="14"/>
-      <c r="Z75" s="31"/>
-      <c r="AB75" s="6"/>
-    </row>
-    <row r="76" spans="1:32" s="31" customFormat="1">
+      <c r="T75" s="32"/>
+      <c r="U75" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V75" s="14"/>
+      <c r="X75" s="31"/>
+      <c r="Z75" s="6"/>
+    </row>
+    <row r="76" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10"/>
       <c r="B76" s="22" t="s">
         <v>94</v>
@@ -5863,23 +5658,19 @@
       <c r="P76" s="34">
         <v>1</v>
       </c>
-      <c r="Q76" s="34">
-        <v>1</v>
-      </c>
+      <c r="Q76" s="34"/>
       <c r="R76" s="34"/>
       <c r="S76" s="34"/>
-      <c r="T76" s="34"/>
-      <c r="U76" s="34"/>
-      <c r="V76" s="32"/>
-      <c r="W76" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X76" s="14"/>
-      <c r="Y76" s="3"/>
-      <c r="AB76" s="6"/>
-    </row>
-    <row r="77" spans="1:32">
+      <c r="T76" s="32"/>
+      <c r="U76" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V76" s="14"/>
+      <c r="W76" s="3"/>
+      <c r="Z76" s="6"/>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B77" s="22" t="s">
         <v>177</v>
       </c>
@@ -5893,18 +5684,18 @@
       <c r="N77" s="34">
         <v>1</v>
       </c>
-      <c r="V77" s="32"/>
-      <c r="W77" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X77" s="14"/>
+      <c r="T77" s="32"/>
+      <c r="U77" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V77" s="14"/>
+      <c r="AA77" s="6"/>
+      <c r="AB77" s="6"/>
       <c r="AC77" s="6"/>
       <c r="AD77" s="6"/>
-      <c r="AE77" s="6"/>
-      <c r="AF77" s="6"/>
-    </row>
-    <row r="78" spans="1:32">
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B78" s="22" t="s">
         <v>95</v>
       </c>
@@ -5935,17 +5726,14 @@
       <c r="P78" s="34">
         <v>1</v>
       </c>
-      <c r="Q78" s="34">
-        <v>1</v>
-      </c>
-      <c r="V78" s="32"/>
-      <c r="W78" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X78" s="14"/>
-    </row>
-    <row r="79" spans="1:32" s="6" customFormat="1">
+      <c r="T78" s="32"/>
+      <c r="U78" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V78" s="14"/>
+    </row>
+    <row r="79" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="10"/>
       <c r="B79" s="22" t="s">
         <v>96</v>
@@ -5980,32 +5768,28 @@
       <c r="P79" s="34">
         <v>1</v>
       </c>
-      <c r="Q79" s="34">
-        <v>1</v>
-      </c>
+      <c r="Q79" s="34"/>
       <c r="R79" s="34"/>
       <c r="S79" s="34"/>
-      <c r="T79" s="34"/>
-      <c r="U79" s="34"/>
-      <c r="V79" s="32"/>
-      <c r="W79" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X79" s="14"/>
-      <c r="Y79" s="3"/>
+      <c r="T79" s="32"/>
+      <c r="U79" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V79" s="14"/>
+      <c r="W79" s="3"/>
+      <c r="X79"/>
+      <c r="Y79"/>
       <c r="Z79"/>
       <c r="AA79"/>
       <c r="AB79"/>
       <c r="AC79"/>
       <c r="AD79"/>
-      <c r="AE79"/>
-      <c r="AF79"/>
-    </row>
-    <row r="80" spans="1:32" s="6" customFormat="1">
+    </row>
+    <row r="80" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="10"/>
       <c r="B80" s="22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C80" s="13">
         <v>1</v>
@@ -6018,7 +5802,7 @@
       <c r="G80" s="13"/>
       <c r="H80" s="13"/>
       <c r="I80" s="21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J80" s="34"/>
       <c r="K80" s="34"/>
@@ -6026,30 +5810,28 @@
       <c r="M80" s="34"/>
       <c r="N80" s="34"/>
       <c r="O80" s="34"/>
-      <c r="P80" s="34"/>
-      <c r="Q80" s="34">
-        <v>1</v>
-      </c>
+      <c r="P80" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q80" s="34"/>
       <c r="R80" s="34"/>
       <c r="S80" s="34"/>
-      <c r="T80" s="34"/>
-      <c r="U80" s="34"/>
-      <c r="V80" s="32"/>
-      <c r="W80" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X80" s="14"/>
-      <c r="Y80" s="3"/>
+      <c r="T80" s="32"/>
+      <c r="U80" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V80" s="14"/>
+      <c r="W80" s="3"/>
+      <c r="X80" s="31"/>
+      <c r="Y80" s="31"/>
       <c r="Z80" s="31"/>
       <c r="AA80" s="31"/>
       <c r="AB80" s="31"/>
       <c r="AC80" s="31"/>
       <c r="AD80" s="31"/>
-      <c r="AE80" s="31"/>
-      <c r="AF80" s="31"/>
-    </row>
-    <row r="81" spans="1:32">
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B81" s="23" t="s">
         <v>97</v>
       </c>
@@ -6077,28 +5859,25 @@
         <v>1</v>
       </c>
       <c r="P81" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q81" s="35">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q81" s="35"/>
       <c r="R81" s="35"/>
       <c r="S81" s="35"/>
       <c r="T81" s="35"/>
-      <c r="U81" s="35"/>
-      <c r="V81" s="35"/>
-      <c r="W81" s="72">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X81" s="14"/>
-    </row>
-    <row r="82" spans="1:32" ht="15" thickBot="1">
+      <c r="U81" s="72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V81" s="14"/>
+    </row>
+    <row r="82" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="11"/>
-      <c r="X82" s="14"/>
-      <c r="AA82" s="31"/>
-    </row>
-    <row r="83" spans="1:32">
+      <c r="U82" s="82"/>
+      <c r="V82" s="14"/>
+      <c r="Y82" s="31"/>
+    </row>
+    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I83" s="61" t="s">
         <v>98</v>
       </c>
@@ -6108,26 +5887,24 @@
       <c r="M83" s="62"/>
       <c r="N83" s="62"/>
       <c r="O83" s="62"/>
-      <c r="P83" s="62"/>
+      <c r="P83" s="62">
+        <f t="array" ref="P83">SUM($C2:$C81*(P2:P81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
+        <v>148</v>
+      </c>
       <c r="Q83" s="62">
-        <f t="array" ref="Q83">SUM($C2:$C81*(Q2:Q81&gt;=0.9)*($W2:$W81&gt;=$Y$12))</f>
-        <v>148</v>
-      </c>
-      <c r="R83" s="62">
-        <f t="array" ref="R83">SUM($C2:$C81*(R2:R81&gt;=0.9)*($W2:$W81&gt;=$Y$12))</f>
+        <f t="array" ref="Q83">SUM($C2:$C81*(Q2:Q81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
         <v>104</v>
       </c>
+      <c r="R83" s="62"/>
       <c r="S83" s="62"/>
-      <c r="T83" s="62"/>
-      <c r="U83" s="62"/>
-      <c r="V83" s="63"/>
-      <c r="X83" s="14"/>
+      <c r="T83" s="63"/>
+      <c r="V83" s="14"/>
+      <c r="AA83" s="6"/>
+      <c r="AB83" s="6"/>
       <c r="AC83" s="6"/>
       <c r="AD83" s="6"/>
-      <c r="AE83" s="6"/>
-      <c r="AF83" s="6"/>
-    </row>
-    <row r="84" spans="1:32">
+    </row>
+    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I84" s="64" t="s">
         <v>100</v>
       </c>
@@ -6137,22 +5914,20 @@
       <c r="M84" s="65"/>
       <c r="N84" s="65"/>
       <c r="O84" s="65"/>
-      <c r="P84" s="65"/>
+      <c r="P84" s="65">
+        <f t="array" ref="P84">SUM($C2:$C81*P2:P81*($U2:$U81&gt;=$W$12))</f>
+        <v>152</v>
+      </c>
       <c r="Q84" s="65">
-        <f t="array" ref="Q84">SUM($C2:$C81*Q2:Q81*($W2:$W81&gt;=$Y$12))</f>
-        <v>153.5</v>
-      </c>
-      <c r="R84" s="65">
-        <f t="array" ref="R84">SUM($C2:$C81*R2:R81*($W2:$W81&gt;=$Y$12))</f>
+        <f t="array" ref="Q84">SUM($C2:$C81*Q2:Q81*($U2:$U81&gt;=$W$12))</f>
         <v>104</v>
       </c>
+      <c r="R84" s="65"/>
       <c r="S84" s="65"/>
-      <c r="T84" s="65"/>
-      <c r="U84" s="65"/>
-      <c r="V84" s="66"/>
-      <c r="X84" s="14"/>
-    </row>
-    <row r="85" spans="1:32" s="6" customFormat="1">
+      <c r="T84" s="66"/>
+      <c r="V84" s="14"/>
+    </row>
+    <row r="85" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10"/>
       <c r="B85" s="22"/>
       <c r="C85" s="13"/>
@@ -6170,31 +5945,29 @@
       <c r="M85" s="65"/>
       <c r="N85" s="65"/>
       <c r="O85" s="65"/>
-      <c r="P85" s="65"/>
+      <c r="P85" s="65">
+        <f t="array" ref="P85">SUM($C$2:$C$81*(P$2:P$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
+        <v>156</v>
+      </c>
       <c r="Q85" s="65">
-        <f t="array" ref="Q85">SUM($C$2:$C$81*(Q$2:Q$81&gt;=0.1)*($W$2:$W$81&gt;=$Y$12))</f>
-        <v>159</v>
-      </c>
-      <c r="R85" s="65">
-        <f t="array" ref="R85">SUM($C$2:$C$81*(R$2:R$81&gt;=0.1)*($W$2:$W$81&gt;=$Y$12))</f>
+        <f t="array" ref="Q85">SUM($C$2:$C$81*(Q$2:Q$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
         <v>104</v>
       </c>
+      <c r="R85" s="65"/>
       <c r="S85" s="65"/>
-      <c r="T85" s="65"/>
-      <c r="U85" s="65"/>
-      <c r="V85" s="66"/>
+      <c r="T85" s="66"/>
+      <c r="U85" s="3"/>
+      <c r="V85" s="14"/>
       <c r="W85" s="3"/>
-      <c r="X85" s="14"/>
-      <c r="Y85" s="3"/>
+      <c r="X85"/>
+      <c r="Y85"/>
       <c r="Z85"/>
       <c r="AA85"/>
       <c r="AB85"/>
       <c r="AC85"/>
       <c r="AD85"/>
-      <c r="AE85"/>
-      <c r="AF85"/>
-    </row>
-    <row r="86" spans="1:32">
+    </row>
+    <row r="86" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I86" s="64" t="s">
         <v>101</v>
       </c>
@@ -6204,26 +5977,24 @@
       <c r="M86" s="65"/>
       <c r="N86" s="65"/>
       <c r="O86" s="65"/>
-      <c r="P86" s="65"/>
+      <c r="P86" s="65">
+        <f t="shared" ref="P86:Q86" si="3">LOOKUP($W$12,$W23:$W31,$X23:$X31)</f>
+        <v>177</v>
+      </c>
       <c r="Q86" s="65">
-        <f t="shared" ref="Q86:R86" si="5">LOOKUP($Y$12,$Y23:$Y31,$Z23:$Z31)</f>
-        <v>180</v>
-      </c>
-      <c r="R86" s="65">
-        <f t="shared" si="5"/>
-        <v>180</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>177</v>
+      </c>
+      <c r="R86" s="65"/>
       <c r="S86" s="65"/>
-      <c r="T86" s="65"/>
-      <c r="U86" s="65"/>
-      <c r="V86" s="66"/>
-      <c r="X86" s="14"/>
+      <c r="T86" s="66"/>
+      <c r="V86" s="14"/>
+      <c r="AA86" s="6"/>
+      <c r="AB86" s="6"/>
       <c r="AC86" s="6"/>
       <c r="AD86" s="6"/>
-      <c r="AE86" s="6"/>
-      <c r="AF86" s="6"/>
-    </row>
-    <row r="87" spans="1:32">
+    </row>
+    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I87" s="64" t="s">
         <v>102</v>
       </c>
@@ -6233,22 +6004,20 @@
       <c r="M87" s="67"/>
       <c r="N87" s="67"/>
       <c r="O87" s="67"/>
-      <c r="P87" s="67"/>
+      <c r="P87" s="67">
+        <f t="shared" ref="P87:Q87" si="4">P84/P86</f>
+        <v>0.85875706214689262</v>
+      </c>
       <c r="Q87" s="67">
-        <f t="shared" ref="Q87:R87" si="6">Q84/Q86</f>
-        <v>0.85277777777777775</v>
-      </c>
-      <c r="R87" s="67">
-        <f t="shared" si="6"/>
-        <v>0.57777777777777772</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>0.58757062146892658</v>
+      </c>
+      <c r="R87" s="67"/>
       <c r="S87" s="67"/>
-      <c r="T87" s="67"/>
-      <c r="U87" s="67"/>
-      <c r="V87" s="68"/>
-      <c r="X87" s="14"/>
-    </row>
-    <row r="88" spans="1:32" ht="15" thickBot="1">
+      <c r="T87" s="68"/>
+      <c r="V87" s="14"/>
+    </row>
+    <row r="88" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C88" s="31"/>
       <c r="I88" s="69" t="s">
         <v>80</v>
@@ -6259,78 +6028,76 @@
       <c r="M88" s="70"/>
       <c r="N88" s="70"/>
       <c r="O88" s="70"/>
-      <c r="P88" s="70"/>
+      <c r="P88" s="70">
+        <f t="shared" ref="P88:Q88" si="5">P86-P84</f>
+        <v>25</v>
+      </c>
       <c r="Q88" s="70">
-        <f t="shared" ref="Q88:R88" si="7">Q86-Q84</f>
-        <v>26.5</v>
-      </c>
-      <c r="R88" s="70">
-        <f t="shared" si="7"/>
-        <v>76</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="R88" s="70"/>
       <c r="S88" s="70"/>
-      <c r="T88" s="70"/>
-      <c r="U88" s="70"/>
-      <c r="V88" s="71"/>
-      <c r="X88" s="14"/>
+      <c r="T88" s="71"/>
+      <c r="V88" s="14"/>
+      <c r="AA88" s="6"/>
+      <c r="AB88" s="6"/>
       <c r="AC88" s="6"/>
       <c r="AD88" s="6"/>
-      <c r="AE88" s="6"/>
-      <c r="AF88" s="6"/>
-    </row>
-    <row r="89" spans="1:32">
+    </row>
+    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C89" s="31"/>
-      <c r="X89" s="14"/>
-    </row>
-    <row r="90" spans="1:32">
+      <c r="V89" s="14"/>
+    </row>
+    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C90" s="31"/>
       <c r="I90" s="13"/>
       <c r="J90" s="13"/>
       <c r="K90" s="13"/>
-      <c r="X90" s="14"/>
-    </row>
-    <row r="91" spans="1:32">
+      <c r="V90" s="14"/>
+    </row>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C91" s="31"/>
       <c r="I91" s="13"/>
       <c r="J91" s="13"/>
       <c r="K91" s="13"/>
-      <c r="X91" s="14"/>
-    </row>
-    <row r="92" spans="1:32">
+      <c r="V91" s="14"/>
+    </row>
+    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I92" s="13"/>
       <c r="J92" s="13"/>
       <c r="K92" s="13"/>
-      <c r="X92" s="14"/>
-    </row>
-    <row r="93" spans="1:32">
+      <c r="V92" s="14"/>
+    </row>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I93" s="13"/>
       <c r="J93" s="13"/>
       <c r="K93" s="13"/>
-      <c r="X93" s="14"/>
-      <c r="AB93" s="31"/>
-    </row>
-    <row r="94" spans="1:32">
+      <c r="V93" s="14"/>
+      <c r="Z93" s="31"/>
+    </row>
+    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I94" s="13"/>
       <c r="J94" s="13"/>
       <c r="K94" s="13"/>
-      <c r="X94" s="14"/>
-    </row>
-    <row r="95" spans="1:32">
+      <c r="V94" s="14"/>
+    </row>
+    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I95" s="13"/>
       <c r="J95" s="13"/>
       <c r="K95" s="13"/>
     </row>
-    <row r="96" spans="1:32">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I96" s="13"/>
       <c r="J96" s="13"/>
       <c r="K96" s="13"/>
     </row>
-    <row r="97" spans="1:32">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.3">
       <c r="I97" s="13"/>
       <c r="J97" s="13"/>
       <c r="K97" s="13"/>
     </row>
-    <row r="98" spans="1:32" s="31" customFormat="1">
+    <row r="98" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="10"/>
       <c r="B98" s="22"/>
       <c r="C98" s="13"/>
@@ -6350,54 +6117,52 @@
       <c r="Q98" s="34"/>
       <c r="R98" s="34"/>
       <c r="S98" s="34"/>
-      <c r="T98" s="34"/>
-      <c r="U98" s="34"/>
-      <c r="V98" s="2"/>
+      <c r="T98" s="2"/>
+      <c r="U98" s="3"/>
+      <c r="V98" s="3"/>
       <c r="W98" s="3"/>
-      <c r="X98" s="3"/>
-      <c r="Y98" s="3"/>
+      <c r="X98"/>
+      <c r="Y98"/>
       <c r="Z98"/>
       <c r="AA98"/>
       <c r="AB98"/>
       <c r="AC98"/>
       <c r="AD98"/>
-      <c r="AE98"/>
-      <c r="AF98"/>
-    </row>
-    <row r="101" spans="1:32">
+    </row>
+    <row r="101" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA101" s="6"/>
+      <c r="AB101" s="6"/>
       <c r="AC101" s="6"/>
       <c r="AD101" s="6"/>
-      <c r="AE101" s="6"/>
-      <c r="AF101" s="6"/>
-    </row>
-    <row r="105" spans="1:32">
+    </row>
+    <row r="105" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA105" s="6"/>
+      <c r="AB105" s="6"/>
       <c r="AC105" s="6"/>
       <c r="AD105" s="6"/>
-      <c r="AE105" s="6"/>
-      <c r="AF105" s="6"/>
-    </row>
-    <row r="110" spans="1:32">
+    </row>
+    <row r="110" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA110" s="6"/>
+      <c r="AB110" s="6"/>
       <c r="AC110" s="6"/>
       <c r="AD110" s="6"/>
-      <c r="AE110" s="6"/>
-      <c r="AF110" s="6"/>
-    </row>
-    <row r="123" spans="29:32">
+    </row>
+    <row r="123" spans="27:30" x14ac:dyDescent="0.3">
+      <c r="AA123" s="31"/>
+      <c r="AB123" s="31"/>
       <c r="AC123" s="31"/>
       <c r="AD123" s="31"/>
-      <c r="AE123" s="31"/>
-      <c r="AF123" s="31"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:W81">
-    <cfRule type="expression" dxfId="2" priority="43" stopIfTrue="1">
-      <formula>$W2&gt;=(0.5+$Y$12)</formula>
+  <conditionalFormatting sqref="B2:U81">
+    <cfRule type="expression" dxfId="2" priority="49" stopIfTrue="1">
+      <formula>$U2&gt;=(0.5+$W$12)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="44" stopIfTrue="1">
-      <formula>$W2&gt;=$Y$12</formula>
+    <cfRule type="expression" dxfId="1" priority="50" stopIfTrue="1">
+      <formula>$U2&gt;=$W$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="45">
-      <formula>$W2&gt;=($Y$12-0.5)</formula>
+    <cfRule type="expression" dxfId="0" priority="51">
+      <formula>$U2&gt;=($W$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6412,379 +6177,379 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A73"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
       <selection sqref="A1:A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>

</xml_diff>